<commit_message>
Did more 2021 predictions, implemented probability value for predictions, created new prediciton maps using that probability threshold.
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA1979F-7EB2-445C-9732-6C9ABBD81107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0DD7C8-BBF7-4622-9F4B-012044EA6C2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="49">
   <si>
     <t>TP</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>T1 V5</t>
+  </si>
+  <si>
+    <t>Matches on Prediction Value</t>
+  </si>
+  <si>
+    <t>Matches on Probability Cut (.75)</t>
+  </si>
+  <si>
+    <t>Matches on Probability Cut (.60)</t>
   </si>
 </sst>
 </file>
@@ -267,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -299,6 +308,11 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +635,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,25 +652,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="A1" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
       <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
@@ -677,26 +681,24 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="15">
-        <v>20.29032258064516</v>
-      </c>
-      <c r="C2" s="15">
-        <v>42.322580645161288</v>
-      </c>
-      <c r="D2" s="15">
-        <v>4123.8709677419356</v>
-      </c>
-      <c r="E2" s="15">
-        <v>265.90322580645159</v>
-      </c>
-      <c r="F2" s="16">
-        <v>32.600927715540323</v>
-      </c>
-      <c r="G2" s="16">
-        <v>93.959153823863247</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>8</v>
@@ -718,26 +720,26 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="11">
-        <v>34.774193548387096</v>
-      </c>
-      <c r="C3" s="11">
-        <v>27.838709677419356</v>
-      </c>
-      <c r="D3" s="11">
-        <v>3691.6774193548385</v>
-      </c>
-      <c r="E3" s="11">
-        <v>698.09677419354841</v>
-      </c>
-      <c r="F3" s="12">
-        <v>55.878254632588273</v>
-      </c>
-      <c r="G3" s="12">
-        <v>84.119319299439553</v>
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="15">
+        <v>20.29032258064516</v>
+      </c>
+      <c r="C3" s="15">
+        <v>42.322580645161288</v>
+      </c>
+      <c r="D3" s="15">
+        <v>4123.8709677419356</v>
+      </c>
+      <c r="E3" s="15">
+        <v>265.90322580645159</v>
+      </c>
+      <c r="F3" s="16">
+        <v>32.600927715540323</v>
+      </c>
+      <c r="G3" s="16">
+        <v>93.959153823863247</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>9</v>
@@ -759,26 +761,26 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="19">
-        <v>34.612903225806448</v>
-      </c>
-      <c r="C4" s="19">
-        <v>28</v>
-      </c>
-      <c r="D4" s="19">
-        <v>3701.0322580645161</v>
-      </c>
-      <c r="E4" s="19">
-        <v>688.74193548387098</v>
-      </c>
-      <c r="F4" s="20">
-        <v>55.668690176865347</v>
-      </c>
-      <c r="G4" s="20">
-        <v>84.331769182202279</v>
+      <c r="A4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="11">
+        <v>34.774193548387096</v>
+      </c>
+      <c r="C4" s="11">
+        <v>27.838709677419356</v>
+      </c>
+      <c r="D4" s="11">
+        <v>3691.6774193548385</v>
+      </c>
+      <c r="E4" s="11">
+        <v>698.09677419354841</v>
+      </c>
+      <c r="F4" s="12">
+        <v>55.878254632588273</v>
+      </c>
+      <c r="G4" s="12">
+        <v>84.119319299439553</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>10</v>
@@ -800,26 +802,26 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="22">
-        <v>21.096774193548388</v>
-      </c>
-      <c r="C5" s="22">
-        <v>41.516129032258064</v>
-      </c>
-      <c r="D5" s="22">
-        <v>4108.8064516129034</v>
-      </c>
-      <c r="E5" s="22">
-        <v>280.96774193548384</v>
-      </c>
-      <c r="F5" s="23">
-        <v>33.553710189901118</v>
-      </c>
-      <c r="G5" s="23">
-        <v>93.608558715329409</v>
+      <c r="A5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="19">
+        <v>34.612903225806448</v>
+      </c>
+      <c r="C5" s="19">
+        <v>28</v>
+      </c>
+      <c r="D5" s="19">
+        <v>3701.0322580645161</v>
+      </c>
+      <c r="E5" s="19">
+        <v>688.74193548387098</v>
+      </c>
+      <c r="F5" s="20">
+        <v>55.668690176865347</v>
+      </c>
+      <c r="G5" s="20">
+        <v>84.331769182202279</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>11</v>
@@ -841,26 +843,26 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="27">
-        <v>35.741935483870968</v>
-      </c>
-      <c r="C6" s="27">
-        <v>26.870967741935484</v>
-      </c>
-      <c r="D6" s="27">
-        <v>3672.0322580645161</v>
-      </c>
-      <c r="E6" s="27">
-        <v>717.74193548387098</v>
-      </c>
-      <c r="F6" s="28">
-        <v>57.379252807455181</v>
-      </c>
-      <c r="G6" s="28">
-        <v>83.673917711123906</v>
+      <c r="A6" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="22">
+        <v>21.096774193548388</v>
+      </c>
+      <c r="C6" s="22">
+        <v>41.516129032258064</v>
+      </c>
+      <c r="D6" s="22">
+        <v>4108.8064516129034</v>
+      </c>
+      <c r="E6" s="22">
+        <v>280.96774193548384</v>
+      </c>
+      <c r="F6" s="23">
+        <v>33.553710189901118</v>
+      </c>
+      <c r="G6" s="23">
+        <v>93.608558715329409</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>12</v>
@@ -882,6 +884,27 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="27">
+        <v>35.741935483870968</v>
+      </c>
+      <c r="C7" s="27">
+        <v>26.870967741935484</v>
+      </c>
+      <c r="D7" s="27">
+        <v>3672.0322580645161</v>
+      </c>
+      <c r="E7" s="27">
+        <v>717.74193548387098</v>
+      </c>
+      <c r="F7" s="28">
+        <v>57.379252807455181</v>
+      </c>
+      <c r="G7" s="28">
+        <v>83.673917711123906</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>13</v>
       </c>
@@ -942,6 +965,15 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
       <c r="J10" s="1" t="s">
         <v>16</v>
       </c>
@@ -962,6 +994,25 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
@@ -982,6 +1033,27 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="32">
+        <v>8.258064516129032</v>
+      </c>
+      <c r="C12" s="32">
+        <v>42.322580645161288</v>
+      </c>
+      <c r="D12" s="32">
+        <v>4123.8709677419356</v>
+      </c>
+      <c r="E12" s="32">
+        <v>82.516129032258064</v>
+      </c>
+      <c r="F12" s="33">
+        <v>13.450995359576535</v>
+      </c>
+      <c r="G12" s="33">
+        <v>91.643043251632392</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1002,6 +1074,27 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="11">
+        <v>19.612903225806452</v>
+      </c>
+      <c r="C13" s="11">
+        <v>27.838709677419356</v>
+      </c>
+      <c r="D13" s="11">
+        <v>3691.6774193548385</v>
+      </c>
+      <c r="E13" s="11">
+        <v>234.19354838709677</v>
+      </c>
+      <c r="F13" s="12">
+        <v>41.262232681707452</v>
+      </c>
+      <c r="G13" s="12">
+        <v>93.986092885169796</v>
+      </c>
       <c r="J13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1022,6 +1115,27 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="19">
+        <v>19.612903225806452</v>
+      </c>
+      <c r="C14" s="19">
+        <v>28</v>
+      </c>
+      <c r="D14" s="19">
+        <v>3701.0322580645161</v>
+      </c>
+      <c r="E14" s="19">
+        <v>231.29032258064515</v>
+      </c>
+      <c r="F14" s="20">
+        <v>41.160181522817055</v>
+      </c>
+      <c r="G14" s="20">
+        <v>94.073266629276389</v>
+      </c>
       <c r="J14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1042,6 +1156,27 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="22">
+        <v>10.483870967741936</v>
+      </c>
+      <c r="C15" s="22">
+        <v>41.516129032258064</v>
+      </c>
+      <c r="D15" s="22">
+        <v>4108.8064516129034</v>
+      </c>
+      <c r="E15" s="22">
+        <v>96.58064516129032</v>
+      </c>
+      <c r="F15" s="23">
+        <v>20.018360072795438</v>
+      </c>
+      <c r="G15" s="23">
+        <v>97.700787205605835</v>
+      </c>
       <c r="J15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1062,6 +1197,27 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="27">
+        <v>18.29032258064516</v>
+      </c>
+      <c r="C16" s="27">
+        <v>26.870967741935484</v>
+      </c>
+      <c r="D16" s="27">
+        <v>3672.0322580645161</v>
+      </c>
+      <c r="E16" s="27">
+        <v>212.35483870967741</v>
+      </c>
+      <c r="F16" s="28">
+        <v>40.674392402180452</v>
+      </c>
+      <c r="G16" s="28">
+        <v>94.491540903388298</v>
+      </c>
       <c r="J16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1081,7 +1237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1101,7 +1257,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1121,7 +1277,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
       <c r="J19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1306,26 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="J20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1161,7 +1345,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="32">
+        <v>15.129032258064516</v>
+      </c>
+      <c r="C21" s="32">
+        <v>42.322580645161288</v>
+      </c>
+      <c r="D21" s="32">
+        <v>4123.8709677419356</v>
+      </c>
+      <c r="E21" s="32">
+        <v>170.61290322580646</v>
+      </c>
+      <c r="F21" s="33">
+        <v>26.526041854582267</v>
+      </c>
+      <c r="G21" s="33">
+        <v>96.025063893420878</v>
+      </c>
       <c r="J21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1181,7 +1386,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="11">
+        <v>29.580645161290324</v>
+      </c>
+      <c r="C22" s="11">
+        <v>27.838709677419356</v>
+      </c>
+      <c r="D22" s="11">
+        <v>3691.6774193548385</v>
+      </c>
+      <c r="E22" s="11">
+        <v>458.67741935483872</v>
+      </c>
+      <c r="F22" s="12">
+        <v>51.675260768234587</v>
+      </c>
+      <c r="G22" s="12">
+        <v>88.902699763653771</v>
+      </c>
       <c r="J22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1201,7 +1427,28 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="19">
+        <v>29.387096774193548</v>
+      </c>
+      <c r="C23" s="19">
+        <v>28</v>
+      </c>
+      <c r="D23" s="19">
+        <v>3701.0322580645161</v>
+      </c>
+      <c r="E23" s="19">
+        <v>451.64516129032256</v>
+      </c>
+      <c r="F23" s="20">
+        <v>51.480031358099119</v>
+      </c>
+      <c r="G23" s="20">
+        <v>89.080991906950146</v>
+      </c>
       <c r="J23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1221,7 +1468,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="22">
+        <v>16.64516129032258</v>
+      </c>
+      <c r="C24" s="22">
+        <v>41.516129032258064</v>
+      </c>
+      <c r="D24" s="22">
+        <v>4108.8064516129034</v>
+      </c>
+      <c r="E24" s="22">
+        <v>186.2258064516129</v>
+      </c>
+      <c r="F24" s="23">
+        <v>28.418568615288478</v>
+      </c>
+      <c r="G24" s="23">
+        <v>95.664189678927968</v>
+      </c>
       <c r="J24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1241,7 +1509,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="27">
+        <v>28.483870967741936</v>
+      </c>
+      <c r="C25" s="27">
+        <v>26.870967741935484</v>
+      </c>
+      <c r="D25" s="27">
+        <v>3672.0322580645161</v>
+      </c>
+      <c r="E25" s="27">
+        <v>436.16129032258067</v>
+      </c>
+      <c r="F25" s="28">
+        <v>51.772562635112131</v>
+      </c>
+      <c r="G25" s="28">
+        <v>89.329116855965751</v>
+      </c>
       <c r="J25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1261,7 +1550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1281,7 +1570,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1301,7 +1590,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1341,7 +1630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1361,7 +1650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1381,7 +1670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1462,6 +1751,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A19:G19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Redid 2021 Predictions with corrected thresholding method. Also added results from implementing distance matching for predictions.
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0DD7C8-BBF7-4622-9F4B-012044EA6C2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6BFFB9-F5FC-4D92-B6CC-D7BBA4F18231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="51">
   <si>
     <t>TP</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Matches on Probability Cut (.60)</t>
+  </si>
+  <si>
+    <t>Matches on Probability Cut (.75) [Distance]</t>
+  </si>
+  <si>
+    <t>Matches on Probability Cut (.60) [Distance]</t>
   </si>
 </sst>
 </file>
@@ -308,11 +314,11 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD331EA-C281-4399-A27A-22CA50F1A7D5}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,40 +653,47 @@
     <col min="5" max="5" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="2" customWidth="1"/>
+    <col min="17" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="J1" s="7" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="Q1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="V1" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -700,26 +713,26 @@
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="T2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="U2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="V2" s="30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
@@ -741,26 +754,26 @@
       <c r="G3" s="16">
         <v>93.959153823863247</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="S3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="T3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="U3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="V3" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>42</v>
       </c>
@@ -782,26 +795,26 @@
       <c r="G4" s="12">
         <v>84.119319299439553</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="S4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="T4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="U4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="V4" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>43</v>
       </c>
@@ -823,26 +836,26 @@
       <c r="G5" s="20">
         <v>84.331769182202279</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="S5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="T5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="U5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="30" t="s">
+      <c r="V5" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>44</v>
       </c>
@@ -864,26 +877,26 @@
       <c r="G6" s="23">
         <v>93.608558715329409</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="R6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="S6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="T6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="U6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="30" t="s">
+      <c r="V6" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>45</v>
       </c>
@@ -905,95 +918,104 @@
       <c r="G7" s="28">
         <v>83.673917711123906</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="R7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="S7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="T7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="U7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="30" t="s">
+      <c r="V7" s="30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J8" s="1" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="S8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="T8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="U8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="30" t="s">
+      <c r="V8" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J9" s="1" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="R9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="S9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="T9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="U9" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="V9" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="J10" s="1" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="I10" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="Q10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="R10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="S10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="T10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="U10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="30" t="s">
+      <c r="V10" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4" t="s">
         <v>0</v>
@@ -1013,67 +1035,107 @@
       <c r="G11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="I11" s="1"/>
+      <c r="J11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="R11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="S11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="T11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="U11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="30" t="s">
+      <c r="V11" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="31">
         <v>8.258064516129032</v>
       </c>
-      <c r="C12" s="32">
-        <v>42.322580645161288</v>
-      </c>
-      <c r="D12" s="32">
-        <v>4123.8709677419356</v>
-      </c>
-      <c r="E12" s="32">
+      <c r="C12" s="31">
+        <v>54.354838709677416</v>
+      </c>
+      <c r="D12" s="31">
+        <v>4307.2580645161288</v>
+      </c>
+      <c r="E12" s="31">
         <v>82.516129032258064</v>
       </c>
-      <c r="F12" s="33">
-        <v>13.450995359576535</v>
-      </c>
-      <c r="G12" s="33">
-        <v>91.643043251632392</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="F12" s="32">
+        <v>9.948874706783613</v>
+      </c>
+      <c r="G12" s="32">
+        <v>91.734324498664066</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="31">
+        <v>13.516129032258064</v>
+      </c>
+      <c r="K12" s="31">
+        <v>54.354838709677416</v>
+      </c>
+      <c r="L12" s="31">
+        <v>4307.2580645161288</v>
+      </c>
+      <c r="M12" s="31">
+        <v>77.258064516129039</v>
+      </c>
+      <c r="N12" s="32">
+        <v>16.264007123870417</v>
+      </c>
+      <c r="O12" s="32">
+        <v>91.851237937386628</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="R12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="S12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="T12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="U12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="30" t="s">
+      <c r="V12" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>42</v>
       </c>
@@ -1081,40 +1143,61 @@
         <v>19.612903225806452</v>
       </c>
       <c r="C13" s="11">
-        <v>27.838709677419356</v>
+        <v>43</v>
       </c>
       <c r="D13" s="11">
-        <v>3691.6774193548385</v>
+        <v>4155.5806451612907</v>
       </c>
       <c r="E13" s="11">
         <v>234.19354838709677</v>
       </c>
       <c r="F13" s="12">
-        <v>41.262232681707452</v>
+        <v>31.002525739692615</v>
       </c>
       <c r="G13" s="12">
-        <v>93.986092885169796</v>
-      </c>
-      <c r="J13" s="1" t="s">
+        <v>94.672148043719787</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="11">
+        <v>32</v>
+      </c>
+      <c r="K13" s="11">
+        <v>43</v>
+      </c>
+      <c r="L13" s="11">
+        <v>4155.5806451612907</v>
+      </c>
+      <c r="M13" s="11">
+        <v>221.80645161290323</v>
+      </c>
+      <c r="N13" s="12">
+        <v>41.619570402166801</v>
+      </c>
+      <c r="O13" s="12">
+        <v>94.939747317059883</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="R13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="S13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="18" t="s">
+      <c r="T13" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="U13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="29" t="s">
+      <c r="V13" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>43</v>
       </c>
@@ -1122,40 +1205,61 @@
         <v>19.612903225806452</v>
       </c>
       <c r="C14" s="19">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D14" s="19">
-        <v>3701.0322580645161</v>
+        <v>4158.4838709677415</v>
       </c>
       <c r="E14" s="19">
         <v>231.29032258064515</v>
       </c>
       <c r="F14" s="20">
-        <v>41.160181522817055</v>
+        <v>30.991664438508739</v>
       </c>
       <c r="G14" s="20">
-        <v>94.073266629276389</v>
-      </c>
-      <c r="J14" s="1" t="s">
+        <v>94.737945400057356</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="19">
+        <v>31.774193548387096</v>
+      </c>
+      <c r="K14" s="19">
+        <v>43</v>
+      </c>
+      <c r="L14" s="19">
+        <v>4158.4838709677415</v>
+      </c>
+      <c r="M14" s="19">
+        <v>219.12903225806451</v>
+      </c>
+      <c r="N14" s="20">
+        <v>41.512148542805434</v>
+      </c>
+      <c r="O14" s="20">
+        <v>95.000837122444139</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="R14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="S14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="18" t="s">
+      <c r="T14" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="U14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="O14" s="29" t="s">
+      <c r="V14" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
@@ -1163,40 +1267,61 @@
         <v>10.483870967741936</v>
       </c>
       <c r="C15" s="22">
-        <v>41.516129032258064</v>
+        <v>52.12903225806452</v>
       </c>
       <c r="D15" s="22">
-        <v>4108.8064516129034</v>
+        <v>4293.1935483870966</v>
       </c>
       <c r="E15" s="22">
         <v>96.58064516129032</v>
       </c>
       <c r="F15" s="23">
-        <v>20.018360072795438</v>
+        <v>16.554420070956912</v>
       </c>
       <c r="G15" s="23">
-        <v>97.700787205605835</v>
-      </c>
-      <c r="J15" s="1" t="s">
+        <v>97.802332919831571</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="22">
+        <v>16.580645161290324</v>
+      </c>
+      <c r="K15" s="22">
+        <v>52.12903225806452</v>
+      </c>
+      <c r="L15" s="22">
+        <v>4293.1935483870966</v>
+      </c>
+      <c r="M15" s="22">
+        <v>90.483870967741936</v>
+      </c>
+      <c r="N15" s="23">
+        <v>23.526332461929584</v>
+      </c>
+      <c r="O15" s="23">
+        <v>97.938116000389286</v>
+      </c>
+      <c r="Q15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="R15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="S15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="18" t="s">
+      <c r="T15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="21" t="s">
+      <c r="U15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="O15" s="14" t="s">
+      <c r="V15" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>45</v>
       </c>
@@ -1204,109 +1329,139 @@
         <v>18.29032258064516</v>
       </c>
       <c r="C16" s="27">
-        <v>26.870967741935484</v>
+        <v>44.322580645161288</v>
       </c>
       <c r="D16" s="27">
-        <v>3672.0322580645161</v>
+        <v>4177.4193548387093</v>
       </c>
       <c r="E16" s="27">
         <v>212.35483870967741</v>
       </c>
       <c r="F16" s="28">
-        <v>40.674392402180452</v>
+        <v>29.072775638698687</v>
       </c>
       <c r="G16" s="28">
-        <v>94.491540903388298</v>
-      </c>
-      <c r="J16" s="1" t="s">
+        <v>95.167460965209429</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="27">
+        <v>29</v>
+      </c>
+      <c r="K16" s="27">
+        <v>44.322580645161288</v>
+      </c>
+      <c r="L16" s="27">
+        <v>4177.4193548387093</v>
+      </c>
+      <c r="M16" s="27">
+        <v>201.64516129032259</v>
+      </c>
+      <c r="N16" s="28">
+        <v>38.941403937810847</v>
+      </c>
+      <c r="O16" s="28">
+        <v>95.399809208465427</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="R16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="S16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="M16" s="18" t="s">
+      <c r="T16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="21" t="s">
+      <c r="U16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="O16" s="14" t="s">
+      <c r="V16" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J17" s="1" t="s">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="R17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="S17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="T17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="24" t="s">
+      <c r="U17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="V17" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J18" s="1" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="R18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="S18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="9" t="s">
+      <c r="T18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N18" s="24" t="s">
+      <c r="U18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="V18" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="J19" s="1" t="s">
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="I19" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="Q19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="R19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="14" t="s">
+      <c r="S19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="9" t="s">
+      <c r="T19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="14" t="s">
+      <c r="U19" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="V19" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
         <v>0</v>
@@ -1326,67 +1481,107 @@
       <c r="G20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="I20" s="1"/>
+      <c r="J20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="R20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="9" t="s">
+      <c r="S20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="T20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="U20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="O20" s="14" t="s">
+      <c r="V20" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="31">
         <v>15.129032258064516</v>
       </c>
-      <c r="C21" s="32">
-        <v>42.322580645161288</v>
-      </c>
-      <c r="D21" s="32">
-        <v>4123.8709677419356</v>
-      </c>
-      <c r="E21" s="32">
+      <c r="C21" s="31">
+        <v>47.483870967741936</v>
+      </c>
+      <c r="D21" s="31">
+        <v>4219.1612903225805</v>
+      </c>
+      <c r="E21" s="31">
         <v>170.61290322580646</v>
       </c>
-      <c r="F21" s="33">
-        <v>26.526041854582267</v>
-      </c>
-      <c r="G21" s="33">
-        <v>96.025063893420878</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="F21" s="32">
+        <v>24.285051780971369</v>
+      </c>
+      <c r="G21" s="32">
+        <v>96.123850695622352</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="31">
+        <v>24.580645161290324</v>
+      </c>
+      <c r="K21" s="31">
+        <v>47.483870967741936</v>
+      </c>
+      <c r="L21" s="31">
+        <v>4219.1612903225805</v>
+      </c>
+      <c r="M21" s="31">
+        <v>161.16129032258064</v>
+      </c>
+      <c r="N21" s="32">
+        <v>33.626433603970419</v>
+      </c>
+      <c r="O21" s="32">
+        <v>96.330244941685066</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="R21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="S21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="T21" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="U21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O21" s="14" t="s">
+      <c r="V21" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>42</v>
       </c>
@@ -1394,40 +1589,61 @@
         <v>29.580645161290324</v>
       </c>
       <c r="C22" s="11">
-        <v>27.838709677419356</v>
+        <v>33.032258064516128</v>
       </c>
       <c r="D22" s="11">
-        <v>3691.6774193548385</v>
+        <v>3931.0967741935483</v>
       </c>
       <c r="E22" s="11">
         <v>458.67741935483872</v>
       </c>
       <c r="F22" s="12">
-        <v>51.675260768234587</v>
+        <v>47.547764640064081</v>
       </c>
       <c r="G22" s="12">
-        <v>88.902699763653771</v>
-      </c>
-      <c r="J22" s="1" t="s">
+        <v>89.565034757113253</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="11">
+        <v>47.70967741935484</v>
+      </c>
+      <c r="K22" s="11">
+        <v>33.032258064516128</v>
+      </c>
+      <c r="L22" s="11">
+        <v>3931.0967741935483</v>
+      </c>
+      <c r="M22" s="11">
+        <v>440.54838709677421</v>
+      </c>
+      <c r="N22" s="12">
+        <v>58.29369207139036</v>
+      </c>
+      <c r="O22" s="12">
+        <v>89.936208742781346</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="R22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="S22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="T22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="U22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="14" t="s">
+      <c r="V22" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>43</v>
       </c>
@@ -1435,40 +1651,61 @@
         <v>29.387096774193548</v>
       </c>
       <c r="C23" s="19">
-        <v>28</v>
+        <v>33.225806451612904</v>
       </c>
       <c r="D23" s="19">
-        <v>3701.0322580645161</v>
+        <v>3938.1290322580644</v>
       </c>
       <c r="E23" s="19">
         <v>451.64516129032256</v>
       </c>
       <c r="F23" s="20">
-        <v>51.480031358099119</v>
+        <v>47.211323894703085</v>
       </c>
       <c r="G23" s="20">
-        <v>89.080991906950146</v>
-      </c>
-      <c r="J23" s="1" t="s">
+        <v>89.724401064903972</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="19">
+        <v>47.483870967741936</v>
+      </c>
+      <c r="K23" s="19">
+        <v>33.225806451612904</v>
+      </c>
+      <c r="L23" s="19">
+        <v>3938.1290322580644</v>
+      </c>
+      <c r="M23" s="19">
+        <v>433.54838709677421</v>
+      </c>
+      <c r="N23" s="20">
+        <v>58.104061096483676</v>
+      </c>
+      <c r="O23" s="20">
+        <v>90.095735937709222</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="R23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="S23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="T23" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="U23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O23" s="14" t="s">
+      <c r="V23" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>44</v>
       </c>
@@ -1476,40 +1713,61 @@
         <v>16.64516129032258</v>
       </c>
       <c r="C24" s="22">
-        <v>41.516129032258064</v>
+        <v>45.967741935483872</v>
       </c>
       <c r="D24" s="22">
-        <v>4108.8064516129034</v>
+        <v>4203.5483870967746</v>
       </c>
       <c r="E24" s="22">
         <v>186.2258064516129</v>
       </c>
       <c r="F24" s="23">
-        <v>28.418568615288478</v>
+        <v>26.426215711975974</v>
       </c>
       <c r="G24" s="23">
-        <v>95.664189678927968</v>
-      </c>
-      <c r="J24" s="1" t="s">
+        <v>95.763248189480422</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="22">
+        <v>26.193548387096776</v>
+      </c>
+      <c r="K24" s="22">
+        <v>45.967741935483872</v>
+      </c>
+      <c r="L24" s="22">
+        <v>4203.5483870967746</v>
+      </c>
+      <c r="M24" s="22">
+        <v>176.67741935483872</v>
+      </c>
+      <c r="N24" s="23">
+        <v>35.649381169552804</v>
+      </c>
+      <c r="O24" s="23">
+        <v>95.971620395119416</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="R24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L24" s="14" t="s">
+      <c r="S24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="T24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="N24" s="14" t="s">
+      <c r="U24" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O24" s="14" t="s">
+      <c r="V24" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>45</v>
       </c>
@@ -1517,245 +1775,269 @@
         <v>28.483870967741936</v>
       </c>
       <c r="C25" s="27">
-        <v>26.870967741935484</v>
+        <v>34.12903225806452</v>
       </c>
       <c r="D25" s="27">
-        <v>3672.0322580645161</v>
+        <v>3953.6129032258063</v>
       </c>
       <c r="E25" s="27">
         <v>436.16129032258067</v>
       </c>
       <c r="F25" s="28">
-        <v>51.772562635112131</v>
+        <v>45.614486881540536</v>
       </c>
       <c r="G25" s="28">
-        <v>89.329116855965751</v>
-      </c>
-      <c r="J25" s="1" t="s">
+        <v>90.076380436315659</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="27">
+        <v>46.483870967741936</v>
+      </c>
+      <c r="K25" s="27">
+        <v>34.12903225806452</v>
+      </c>
+      <c r="L25" s="27">
+        <v>3953.6129032258063</v>
+      </c>
+      <c r="M25" s="27">
+        <v>418.16129032258067</v>
+      </c>
+      <c r="N25" s="28">
+        <v>56.900838561911783</v>
+      </c>
+      <c r="O25" s="28">
+        <v>90.447038208706573</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="R25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="S25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="T25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="N25" s="14" t="s">
+      <c r="U25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="14" t="s">
+      <c r="V25" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J26" s="1" t="s">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="R26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="S26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="T26" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="U26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="O26" s="14" t="s">
+      <c r="V26" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="1" t="s">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="R27" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L27" s="14" t="s">
+      <c r="S27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="T27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="N27" s="14" t="s">
+      <c r="U27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="O27" s="14" t="s">
+      <c r="V27" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J28" s="1" t="s">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="R28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="S28" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M28" s="14" t="s">
+      <c r="T28" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="N28" s="14" t="s">
+      <c r="U28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O28" s="14" t="s">
+      <c r="V28" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J29" s="1" t="s">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="R29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L29" s="14" t="s">
+      <c r="S29" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="14" t="s">
+      <c r="T29" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N29" s="14" t="s">
+      <c r="U29" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O29" s="14" t="s">
+      <c r="V29" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J30" s="1" t="s">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="R30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="14" t="s">
+      <c r="S30" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M30" s="14" t="s">
+      <c r="T30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N30" s="14" t="s">
+      <c r="U30" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="O30" s="14" t="s">
+      <c r="V30" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J31" s="1" t="s">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="R31" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L31" s="14" t="s">
+      <c r="S31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="14" t="s">
+      <c r="T31" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="N31" s="14" t="s">
+      <c r="U31" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O31" s="14" t="s">
+      <c r="V31" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J32" s="1" t="s">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="R32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="S32" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="T32" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="N32" s="14" t="s">
+      <c r="U32" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="O32" s="14" t="s">
+      <c r="V32" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J33" s="1" t="s">
+    <row r="33" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="R33" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L33" s="14" t="s">
+      <c r="S33" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="M33" s="14" t="s">
+      <c r="T33" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N33" s="14" t="s">
+      <c r="U33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O33" s="14" t="s">
+      <c r="V33" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J34" s="1" t="s">
+    <row r="34" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K34" s="14" t="s">
+      <c r="R34" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="L34" s="14" t="s">
+      <c r="S34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M34" s="14" t="s">
+      <c r="T34" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="N34" s="14" t="s">
+      <c r="U34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O34" s="14" t="s">
+      <c r="V34" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J35" s="1" t="s">
+    <row r="35" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="14" t="s">
+      <c r="R35" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="14" t="s">
+      <c r="S35" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M35" s="14" t="s">
+      <c r="T35" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="14" t="s">
+      <c r="U35" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="O35" s="14" t="s">
+      <c r="V35" s="14" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A19:G19"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="I19:O19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Redid 2021 predictions, corrected TN and FN values based on matched predictions using distance.
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6BFFB9-F5FC-4D92-B6CC-D7BBA4F18231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DBC2CD-BE2C-4C34-8203-29C29AC5B5D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="53">
   <si>
     <t>TP</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Matches on Probability Cut (.60) [Distance]</t>
+  </si>
+  <si>
+    <t>Matches on Prediction Value [Distance]</t>
+  </si>
+  <si>
+    <t>NTP</t>
   </si>
 </sst>
 </file>
@@ -255,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -278,11 +284,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -316,7 +379,25 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -638,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD331EA-C281-4399-A27A-22CA50F1A7D5}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,39 +742,51 @@
     <col min="13" max="13" width="4.5703125" style="3" customWidth="1"/>
     <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="11.140625" style="2" customWidth="1"/>
-    <col min="17" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="3"/>
+    <col min="18" max="23" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="Q1" s="7" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="I1" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="R1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -713,309 +806,452 @@
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="18" t="s">
+      <c r="U2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="V2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="15">
-        <v>20.29032258064516</v>
+        <v>20.483870967741936</v>
       </c>
       <c r="C3" s="15">
-        <v>42.322580645161288</v>
+        <v>42.12903225806452</v>
       </c>
       <c r="D3" s="15">
-        <v>4123.8709677419356</v>
+        <v>4119.7741935483873</v>
       </c>
       <c r="E3" s="15">
-        <v>265.90322580645159</v>
+        <v>270</v>
       </c>
       <c r="F3" s="16">
-        <v>32.600927715540323</v>
+        <v>32.967421219265887</v>
       </c>
       <c r="G3" s="16">
-        <v>93.959153823863247</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+        <v>93.866326112069842</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="15">
+        <v>28.451612903225808</v>
+      </c>
+      <c r="K3" s="15">
+        <v>34.161290322580648</v>
+      </c>
+      <c r="L3" s="15">
+        <v>4127.7419354838712</v>
+      </c>
+      <c r="M3" s="15">
+        <v>262.03225806451616</v>
+      </c>
+      <c r="N3" s="16">
+        <v>46.117155580882667</v>
+      </c>
+      <c r="O3" s="16">
+        <v>94.04732682027192</v>
+      </c>
+      <c r="P3" s="15">
+        <v>7.967741935483871</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="U3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="V3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="30" t="s">
+      <c r="W3" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="11">
-        <v>34.774193548387096</v>
+        <v>35.064516129032256</v>
       </c>
       <c r="C4" s="11">
-        <v>27.838709677419356</v>
+        <v>27.548387096774192</v>
       </c>
       <c r="D4" s="11">
-        <v>3691.6774193548385</v>
+        <v>3686.7419354838707</v>
       </c>
       <c r="E4" s="11">
-        <v>698.09677419354841</v>
+        <v>703.0322580645161</v>
       </c>
       <c r="F4" s="12">
-        <v>55.878254632588273</v>
+        <v>56.429834936558031</v>
       </c>
       <c r="G4" s="12">
-        <v>84.119319299439553</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+        <v>84.006794528998711</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="11">
+        <v>49.483870967741936</v>
+      </c>
+      <c r="K4" s="11">
+        <v>13.129032258064516</v>
+      </c>
+      <c r="L4" s="11">
+        <v>3701.1612903225805</v>
+      </c>
+      <c r="M4" s="11">
+        <v>688.61290322580646</v>
+      </c>
+      <c r="N4" s="12">
+        <v>80.149309072254894</v>
+      </c>
+      <c r="O4" s="12">
+        <v>84.335056504683791</v>
+      </c>
+      <c r="P4" s="11">
+        <v>14.419354838709678</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="T4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="T4" s="18" t="s">
+      <c r="U4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="V4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="30" t="s">
+      <c r="W4" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="19">
-        <v>34.612903225806448</v>
+        <v>35</v>
       </c>
       <c r="C5" s="19">
-        <v>28</v>
+        <v>27.612903225806452</v>
       </c>
       <c r="D5" s="19">
-        <v>3701.0322580645161</v>
+        <v>3696.2258064516127</v>
       </c>
       <c r="E5" s="19">
-        <v>688.74193548387098</v>
+        <v>693.54838709677415</v>
       </c>
       <c r="F5" s="20">
-        <v>55.668690176865347</v>
+        <v>56.316638665548091</v>
       </c>
       <c r="G5" s="20">
-        <v>84.331769182202279</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+        <v>84.221882132102451</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="19">
+        <v>49.12903225806452</v>
+      </c>
+      <c r="K5" s="19">
+        <v>13.483870967741936</v>
+      </c>
+      <c r="L5" s="19">
+        <v>3710.3548387096776</v>
+      </c>
+      <c r="M5" s="19">
+        <v>679.41935483870964</v>
+      </c>
+      <c r="N5" s="20">
+        <v>79.528640881418781</v>
+      </c>
+      <c r="O5" s="20">
+        <v>84.543564737159983</v>
+      </c>
+      <c r="P5" s="19">
+        <v>14.129032258064516</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="T5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="U5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U5" s="21" t="s">
+      <c r="V5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="V5" s="30" t="s">
+      <c r="W5" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="22">
-        <v>21.096774193548388</v>
+        <v>21.451612903225808</v>
       </c>
       <c r="C6" s="22">
-        <v>41.516129032258064</v>
+        <v>41.161290322580648</v>
       </c>
       <c r="D6" s="22">
-        <v>4108.8064516129034</v>
+        <v>4103.2258064516127</v>
       </c>
       <c r="E6" s="22">
-        <v>280.96774193548384</v>
+        <v>286.54838709677421</v>
       </c>
       <c r="F6" s="23">
-        <v>33.553710189901118</v>
+        <v>34.091820100119499</v>
       </c>
       <c r="G6" s="23">
-        <v>93.608558715329409</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+        <v>93.481193786837395</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="22">
+        <v>29.387096774193548</v>
+      </c>
+      <c r="K6" s="22">
+        <v>33.225806451612904</v>
+      </c>
+      <c r="L6" s="22">
+        <v>4111.1612903225805</v>
+      </c>
+      <c r="M6" s="22">
+        <v>278.61290322580646</v>
+      </c>
+      <c r="N6" s="23">
+        <v>47.182106813471258</v>
+      </c>
+      <c r="O6" s="23">
+        <v>93.661473513021477</v>
+      </c>
+      <c r="P6" s="22">
+        <v>7.935483870967742</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="T6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="18" t="s">
+      <c r="U6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="21" t="s">
+      <c r="V6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="30" t="s">
+      <c r="W6" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="27">
-        <v>35.741935483870968</v>
+        <v>36.258064516129032</v>
       </c>
       <c r="C7" s="27">
-        <v>26.870967741935484</v>
+        <v>26.35483870967742</v>
       </c>
       <c r="D7" s="27">
-        <v>3672.0322580645161</v>
+        <v>3666.2903225806454</v>
       </c>
       <c r="E7" s="27">
-        <v>717.74193548387098</v>
+        <v>723.48387096774195</v>
       </c>
       <c r="F7" s="28">
-        <v>57.379252807455181</v>
+        <v>58.108574742803064</v>
       </c>
       <c r="G7" s="28">
-        <v>83.673917711123906</v>
-      </c>
-      <c r="Q7" s="1" t="s">
+        <v>83.542654648323293</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="27">
+        <v>50.645161290322584</v>
+      </c>
+      <c r="K7" s="27">
+        <v>11.96774193548387</v>
+      </c>
+      <c r="L7" s="27">
+        <v>3680.6774193548385</v>
+      </c>
+      <c r="M7" s="27">
+        <v>709.09677419354841</v>
+      </c>
+      <c r="N7" s="28">
+        <v>81.452345269896909</v>
+      </c>
+      <c r="O7" s="28">
+        <v>83.869996830115056</v>
+      </c>
+      <c r="P7" s="27">
+        <v>14.387096774193548</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="T7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="T7" s="18" t="s">
+      <c r="U7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="21" t="s">
+      <c r="V7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="30" t="s">
+      <c r="W7" s="30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q8" s="1" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="T8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="18" t="s">
+      <c r="U8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="U8" s="21" t="s">
+      <c r="V8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="V8" s="30" t="s">
+      <c r="W8" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q9" s="1" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="T9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="T9" s="18" t="s">
+      <c r="U9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="U9" s="21" t="s">
+      <c r="V9" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="V9" s="30" t="s">
+      <c r="W9" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="I10" s="33" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="I10" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="Q10" s="1" t="s">
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="37"/>
+      <c r="R10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="S10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="T10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="18" t="s">
+      <c r="U10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="U10" s="21" t="s">
+      <c r="V10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="V10" s="30" t="s">
+      <c r="W10" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4" t="s">
         <v>0</v>
@@ -1054,414 +1290,433 @@
       <c r="O11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="P11" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R11" s="6" t="s">
+      <c r="S11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="13" t="s">
+      <c r="T11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="T11" s="18" t="s">
+      <c r="U11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U11" s="21" t="s">
+      <c r="V11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="V11" s="30" t="s">
+      <c r="W11" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="31">
-        <v>8.258064516129032</v>
+        <v>8.3548387096774199</v>
       </c>
       <c r="C12" s="31">
-        <v>54.354838709677416</v>
+        <v>54.258064516129032</v>
       </c>
       <c r="D12" s="31">
-        <v>4307.2580645161288</v>
+        <v>4306.322580645161</v>
       </c>
       <c r="E12" s="31">
-        <v>82.516129032258064</v>
+        <v>83.451612903225808</v>
       </c>
       <c r="F12" s="32">
-        <v>9.948874706783613</v>
+        <v>10.086283732417924</v>
       </c>
       <c r="G12" s="32">
-        <v>91.734324498664066</v>
+        <v>91.715479750131749</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J12" s="31">
-        <v>13.516129032258064</v>
+        <v>11.870967741935484</v>
       </c>
       <c r="K12" s="31">
-        <v>54.354838709677416</v>
+        <v>50.741935483870968</v>
       </c>
       <c r="L12" s="31">
-        <v>4307.2580645161288</v>
+        <v>4309.8387096774195</v>
       </c>
       <c r="M12" s="31">
-        <v>77.258064516129039</v>
+        <v>79.935483870967744</v>
       </c>
       <c r="N12" s="32">
-        <v>16.264007123870417</v>
+        <v>15.913783677093578</v>
       </c>
       <c r="O12" s="32">
-        <v>91.851237937386628</v>
-      </c>
-      <c r="Q12" s="1" t="s">
+        <v>91.795223056364762</v>
+      </c>
+      <c r="P12" s="15">
+        <v>3.5161290322580645</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="S12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="T12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="T12" s="18" t="s">
+      <c r="U12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="U12" s="21" t="s">
+      <c r="V12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="V12" s="30" t="s">
+      <c r="W12" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="11">
-        <v>19.612903225806452</v>
+        <v>19.870967741935484</v>
       </c>
       <c r="C13" s="11">
-        <v>43</v>
+        <v>42.741935483870968</v>
       </c>
       <c r="D13" s="11">
-        <v>4155.5806451612907</v>
+        <v>4150.9677419354839</v>
       </c>
       <c r="E13" s="11">
-        <v>234.19354838709677</v>
+        <v>238.80645161290323</v>
       </c>
       <c r="F13" s="12">
-        <v>31.002525739692615</v>
+        <v>31.432146871392032</v>
       </c>
       <c r="G13" s="12">
-        <v>94.672148043719787</v>
+        <v>94.566913986806313</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="11">
-        <v>32</v>
+        <v>27.64516129032258</v>
       </c>
       <c r="K13" s="11">
-        <v>43</v>
+        <v>34.967741935483872</v>
       </c>
       <c r="L13" s="11">
-        <v>4155.5806451612907</v>
+        <v>4158.7419354838712</v>
       </c>
       <c r="M13" s="11">
-        <v>221.80645161290323</v>
+        <v>231.03225806451613</v>
       </c>
       <c r="N13" s="12">
-        <v>41.619570402166801</v>
+        <v>44.313172788593675</v>
       </c>
       <c r="O13" s="12">
-        <v>94.939747317059883</v>
-      </c>
-      <c r="Q13" s="1" t="s">
+        <v>94.743640199565377</v>
+      </c>
+      <c r="P13" s="11">
+        <v>7.774193548387097</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R13" s="6" t="s">
+      <c r="S13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="T13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T13" s="18" t="s">
+      <c r="U13" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="U13" s="21" t="s">
+      <c r="V13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="V13" s="29" t="s">
+      <c r="W13" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="19">
-        <v>19.612903225806452</v>
+        <v>19.774193548387096</v>
       </c>
       <c r="C14" s="19">
-        <v>43</v>
+        <v>42.838709677419352</v>
       </c>
       <c r="D14" s="19">
-        <v>4158.4838709677415</v>
+        <v>4153.6129032258068</v>
       </c>
       <c r="E14" s="19">
-        <v>231.29032258064515</v>
+        <v>236.16129032258064</v>
       </c>
       <c r="F14" s="20">
-        <v>30.991664438508739</v>
+        <v>31.286727909479879</v>
       </c>
       <c r="G14" s="20">
-        <v>94.737945400057356</v>
+        <v>94.626760916422313</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="19">
-        <v>31.774193548387096</v>
+        <v>27.516129032258064</v>
       </c>
       <c r="K14" s="19">
-        <v>43</v>
+        <v>35.096774193548384</v>
       </c>
       <c r="L14" s="19">
-        <v>4158.4838709677415</v>
+        <v>4161.3548387096771</v>
       </c>
       <c r="M14" s="19">
-        <v>219.12903225806451</v>
+        <v>228.41935483870967</v>
       </c>
       <c r="N14" s="20">
-        <v>41.512148542805434</v>
+        <v>44.131911532774708</v>
       </c>
       <c r="O14" s="20">
-        <v>95.000837122444139</v>
-      </c>
-      <c r="Q14" s="1" t="s">
+        <v>94.802753674846414</v>
+      </c>
+      <c r="P14" s="19">
+        <v>7.741935483870968</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R14" s="6" t="s">
+      <c r="S14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="T14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="T14" s="18" t="s">
+      <c r="U14" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="U14" s="21" t="s">
+      <c r="V14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="V14" s="29" t="s">
+      <c r="W14" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="22">
-        <v>10.483870967741936</v>
+        <v>10.741935483870968</v>
       </c>
       <c r="C15" s="22">
-        <v>52.12903225806452</v>
+        <v>51.87096774193548</v>
       </c>
       <c r="D15" s="22">
-        <v>4293.1935483870966</v>
+        <v>4291.4516129032254</v>
       </c>
       <c r="E15" s="22">
-        <v>96.58064516129032</v>
+        <v>98.322580645161295</v>
       </c>
       <c r="F15" s="23">
-        <v>16.554420070956912</v>
+        <v>17.009450859865115</v>
       </c>
       <c r="G15" s="23">
-        <v>97.802332919831571</v>
+        <v>97.762639665280531</v>
       </c>
       <c r="I15" s="25" t="s">
         <v>44</v>
       </c>
       <c r="J15" s="22">
-        <v>16.580645161290324</v>
+        <v>14.709677419354838</v>
       </c>
       <c r="K15" s="22">
-        <v>52.12903225806452</v>
+        <v>47.903225806451616</v>
       </c>
       <c r="L15" s="22">
-        <v>4293.1935483870966</v>
+        <v>4295.4193548387093</v>
       </c>
       <c r="M15" s="22">
-        <v>90.483870967741936</v>
+        <v>94.354838709677423</v>
       </c>
       <c r="N15" s="23">
-        <v>23.526332461929584</v>
+        <v>23.410546202487399</v>
       </c>
       <c r="O15" s="23">
-        <v>97.938116000389286</v>
-      </c>
-      <c r="Q15" s="1" t="s">
+        <v>97.852913170256514</v>
+      </c>
+      <c r="P15" s="22">
+        <v>3.967741935483871</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="6" t="s">
+      <c r="S15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="S15" s="13" t="s">
+      <c r="T15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T15" s="18" t="s">
+      <c r="U15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="U15" s="21" t="s">
+      <c r="V15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="V15" s="14" t="s">
+      <c r="W15" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="27">
-        <v>18.29032258064516</v>
+        <v>18.903225806451612</v>
       </c>
       <c r="C16" s="27">
-        <v>44.322580645161288</v>
+        <v>43.70967741935484</v>
       </c>
       <c r="D16" s="27">
-        <v>4177.4193548387093</v>
+        <v>4173.1935483870966</v>
       </c>
       <c r="E16" s="27">
-        <v>212.35483870967741</v>
+        <v>216.58064516129033</v>
       </c>
       <c r="F16" s="28">
-        <v>29.072775638698687</v>
+        <v>30.006507510804845</v>
       </c>
       <c r="G16" s="28">
-        <v>95.167460965209429</v>
+        <v>95.071603315232068</v>
       </c>
       <c r="I16" s="26" t="s">
         <v>45</v>
       </c>
       <c r="J16" s="27">
+        <v>25.548387096774192</v>
+      </c>
+      <c r="K16" s="27">
+        <v>37.064516129032256</v>
+      </c>
+      <c r="L16" s="27">
+        <v>4179.8387096774195</v>
+      </c>
+      <c r="M16" s="27">
+        <v>209.93548387096774</v>
+      </c>
+      <c r="N16" s="28">
+        <v>40.892388432441187</v>
+      </c>
+      <c r="O16" s="28">
+        <v>95.222632512794803</v>
+      </c>
+      <c r="P16" s="27">
+        <v>6.645161290322581</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="V16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="V17" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="27">
-        <v>44.322580645161288</v>
-      </c>
-      <c r="L16" s="27">
-        <v>4177.4193548387093</v>
-      </c>
-      <c r="M16" s="27">
-        <v>201.64516129032259</v>
-      </c>
-      <c r="N16" s="28">
-        <v>38.941403937810847</v>
-      </c>
-      <c r="O16" s="28">
-        <v>95.399809208465427</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S16" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="T16" s="18" t="s">
+      <c r="T18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="U16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="V16" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S17" s="13" t="s">
+      <c r="U18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V18" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="I19" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="37"/>
+      <c r="R19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="U19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="U17" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="V17" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q18" s="1" t="s">
+      <c r="W19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="R18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="T18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="U18" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="V18" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="I19" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="Q19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="S19" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="T19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="U19" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="V19" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
         <v>0</v>
@@ -1500,542 +1755,561 @@
       <c r="O20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="P20" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R20" s="6" t="s">
+      <c r="S20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="S20" s="9" t="s">
+      <c r="T20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="T20" s="9" t="s">
+      <c r="U20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="U20" s="14" t="s">
+      <c r="V20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="V20" s="14" t="s">
+      <c r="W20" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="31">
-        <v>15.129032258064516</v>
+        <v>15.193548387096774</v>
       </c>
       <c r="C21" s="31">
-        <v>47.483870967741936</v>
+        <v>47.41935483870968</v>
       </c>
       <c r="D21" s="31">
-        <v>4219.1612903225805</v>
+        <v>4216.1290322580644</v>
       </c>
       <c r="E21" s="31">
-        <v>170.61290322580646</v>
+        <v>173.64516129032259</v>
       </c>
       <c r="F21" s="32">
-        <v>24.285051780971369</v>
+        <v>24.369636715007047</v>
       </c>
       <c r="G21" s="32">
-        <v>96.123850695622352</v>
+        <v>96.055115466237112</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J21" s="31">
-        <v>24.580645161290324</v>
+        <v>21.193548387096776</v>
       </c>
       <c r="K21" s="31">
-        <v>47.483870967741936</v>
+        <v>41.41935483870968</v>
       </c>
       <c r="L21" s="31">
-        <v>4219.1612903225805</v>
+        <v>4222.1290322580644</v>
       </c>
       <c r="M21" s="31">
-        <v>161.16129032258064</v>
+        <v>167.64516129032259</v>
       </c>
       <c r="N21" s="32">
-        <v>33.626433603970419</v>
+        <v>34.433244066226969</v>
       </c>
       <c r="O21" s="32">
-        <v>96.330244941685066</v>
-      </c>
-      <c r="Q21" s="1" t="s">
+        <v>96.19144771472719</v>
+      </c>
+      <c r="P21" s="31">
+        <v>6</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R21" s="6" t="s">
+      <c r="S21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="S21" s="9" t="s">
+      <c r="T21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="T21" s="14" t="s">
+      <c r="U21" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="U21" s="9" t="s">
+      <c r="V21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="V21" s="14" t="s">
+      <c r="W21" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="11">
-        <v>29.580645161290324</v>
+        <v>29.806451612903224</v>
       </c>
       <c r="C22" s="11">
-        <v>33.032258064516128</v>
+        <v>32.806451612903224</v>
       </c>
       <c r="D22" s="11">
-        <v>3931.0967741935483</v>
+        <v>3925.8709677419356</v>
       </c>
       <c r="E22" s="11">
-        <v>458.67741935483872</v>
+        <v>463.90322580645159</v>
       </c>
       <c r="F22" s="12">
-        <v>47.547764640064081</v>
+        <v>47.867886696854754</v>
       </c>
       <c r="G22" s="12">
-        <v>89.565034757113253</v>
+        <v>89.445897020202395</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>42</v>
       </c>
       <c r="J22" s="11">
-        <v>47.70967741935484</v>
+        <v>41</v>
       </c>
       <c r="K22" s="11">
-        <v>33.032258064516128</v>
+        <v>21.612903225806452</v>
       </c>
       <c r="L22" s="11">
-        <v>3931.0967741935483</v>
+        <v>3937.0645161290322</v>
       </c>
       <c r="M22" s="11">
-        <v>440.54838709677421</v>
+        <v>452.70967741935482</v>
       </c>
       <c r="N22" s="12">
-        <v>58.29369207139036</v>
+        <v>66.1974474462789</v>
       </c>
       <c r="O22" s="12">
-        <v>89.936208742781346</v>
-      </c>
-      <c r="Q22" s="1" t="s">
+        <v>89.700721360683744</v>
+      </c>
+      <c r="P22" s="11">
+        <v>11.193548387096774</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R22" s="6" t="s">
+      <c r="S22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S22" s="9" t="s">
+      <c r="T22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T22" s="14" t="s">
+      <c r="U22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="U22" s="9" t="s">
+      <c r="V22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="V22" s="14" t="s">
+      <c r="W22" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="19">
-        <v>29.387096774193548</v>
+        <v>29.677419354838708</v>
       </c>
       <c r="C23" s="19">
-        <v>33.225806451612904</v>
+        <v>32.935483870967744</v>
       </c>
       <c r="D23" s="19">
-        <v>3938.1290322580644</v>
+        <v>3933.2258064516127</v>
       </c>
       <c r="E23" s="19">
-        <v>451.64516129032256</v>
+        <v>456.54838709677421</v>
       </c>
       <c r="F23" s="20">
-        <v>47.211323894703085</v>
+        <v>47.643872512761895</v>
       </c>
       <c r="G23" s="20">
-        <v>89.724401064903972</v>
+        <v>89.612897925432904</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J23" s="19">
-        <v>47.483870967741936</v>
+        <v>40.967741935483872</v>
       </c>
       <c r="K23" s="19">
-        <v>33.225806451612904</v>
+        <v>21.64516129032258</v>
       </c>
       <c r="L23" s="19">
-        <v>3938.1290322580644</v>
+        <v>3944.516129032258</v>
       </c>
       <c r="M23" s="19">
-        <v>433.54838709677421</v>
+        <v>445.25806451612902</v>
       </c>
       <c r="N23" s="20">
-        <v>58.104061096483676</v>
+        <v>66.157139063244443</v>
       </c>
       <c r="O23" s="20">
-        <v>90.095735937709222</v>
-      </c>
-      <c r="Q23" s="1" t="s">
+        <v>89.869914418749701</v>
+      </c>
+      <c r="P23" s="19">
+        <v>11.290322580645162</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R23" s="6" t="s">
+      <c r="S23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S23" s="14" t="s">
+      <c r="T23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="T23" s="14" t="s">
+      <c r="U23" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="U23" s="9" t="s">
+      <c r="V23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="V23" s="14" t="s">
+      <c r="W23" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="22">
-        <v>16.64516129032258</v>
+        <v>17.032258064516128</v>
       </c>
       <c r="C24" s="22">
-        <v>45.967741935483872</v>
+        <v>45.58064516129032</v>
       </c>
       <c r="D24" s="22">
-        <v>4203.5483870967746</v>
+        <v>4199.1935483870966</v>
       </c>
       <c r="E24" s="22">
-        <v>186.2258064516129</v>
+        <v>190.58064516129033</v>
       </c>
       <c r="F24" s="23">
-        <v>26.426215711975974</v>
+        <v>27.121949823522591</v>
       </c>
       <c r="G24" s="23">
-        <v>95.763248189480422</v>
+        <v>95.66381849693002</v>
       </c>
       <c r="I24" s="25" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="22">
-        <v>26.193548387096776</v>
+        <v>23.06451612903226</v>
       </c>
       <c r="K24" s="22">
-        <v>45.967741935483872</v>
+        <v>39.548387096774192</v>
       </c>
       <c r="L24" s="22">
-        <v>4203.5483870967746</v>
+        <v>4205.2258064516127</v>
       </c>
       <c r="M24" s="22">
-        <v>176.67741935483872</v>
+        <v>184.54838709677421</v>
       </c>
       <c r="N24" s="23">
-        <v>35.649381169552804</v>
+        <v>37.01474743980296</v>
       </c>
       <c r="O24" s="23">
-        <v>95.971620395119416</v>
-      </c>
-      <c r="Q24" s="1" t="s">
+        <v>95.800937942331601</v>
+      </c>
+      <c r="P24" s="22">
+        <v>6.032258064516129</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R24" s="6" t="s">
+      <c r="S24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S24" s="14" t="s">
+      <c r="T24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="T24" s="14" t="s">
+      <c r="U24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="U24" s="14" t="s">
+      <c r="V24" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="V24" s="14" t="s">
+      <c r="W24" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="27">
-        <v>28.483870967741936</v>
+        <v>28.903225806451612</v>
       </c>
       <c r="C25" s="27">
-        <v>34.12903225806452</v>
+        <v>33.70967741935484</v>
       </c>
       <c r="D25" s="27">
-        <v>3953.6129032258063</v>
+        <v>3947.516129032258</v>
       </c>
       <c r="E25" s="27">
-        <v>436.16129032258067</v>
+        <v>442.25806451612902</v>
       </c>
       <c r="F25" s="28">
-        <v>45.614486881540536</v>
+        <v>46.313100591954786</v>
       </c>
       <c r="G25" s="28">
-        <v>90.076380436315659</v>
+        <v>89.937514605778802</v>
       </c>
       <c r="I25" s="26" t="s">
         <v>45</v>
       </c>
       <c r="J25" s="27">
-        <v>46.483870967741936</v>
+        <v>39.87096774193548</v>
       </c>
       <c r="K25" s="27">
-        <v>34.12903225806452</v>
+        <v>22.741935483870968</v>
       </c>
       <c r="L25" s="27">
-        <v>3953.6129032258063</v>
+        <v>3958.483870967742</v>
       </c>
       <c r="M25" s="27">
-        <v>418.16129032258067</v>
+        <v>431.29032258064518</v>
       </c>
       <c r="N25" s="28">
-        <v>56.900838561911783</v>
+        <v>64.30291994486133</v>
       </c>
       <c r="O25" s="28">
-        <v>90.447038208706573</v>
-      </c>
-      <c r="Q25" s="1" t="s">
+        <v>90.186976579405197</v>
+      </c>
+      <c r="P25" s="27">
+        <v>10.96774193548387</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R25" s="6" t="s">
+      <c r="S25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="S25" s="14" t="s">
+      <c r="T25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="T25" s="14" t="s">
+      <c r="U25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="U25" s="14" t="s">
+      <c r="V25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="V25" s="14" t="s">
+      <c r="W25" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q26" s="1" t="s">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R26" s="6" t="s">
+      <c r="S26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S26" s="14" t="s">
+      <c r="T26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="14" t="s">
+      <c r="U26" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="U26" s="14" t="s">
+      <c r="V26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="V26" s="14" t="s">
+      <c r="W26" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q27" s="1" t="s">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R27" s="6" t="s">
+      <c r="S27" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="S27" s="14" t="s">
+      <c r="T27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="14" t="s">
+      <c r="U27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="U27" s="14" t="s">
+      <c r="V27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V27" s="14" t="s">
+      <c r="W27" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q28" s="1" t="s">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R28" s="6" t="s">
+      <c r="S28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="S28" s="14" t="s">
+      <c r="T28" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="T28" s="14" t="s">
+      <c r="U28" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="U28" s="14" t="s">
+      <c r="V28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="V28" s="14" t="s">
+      <c r="W28" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q29" s="1" t="s">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R29" s="6" t="s">
+      <c r="S29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="S29" s="14" t="s">
+      <c r="T29" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="T29" s="14" t="s">
+      <c r="U29" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="U29" s="14" t="s">
+      <c r="V29" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="V29" s="14" t="s">
+      <c r="W29" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q30" s="1" t="s">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R30" s="6" t="s">
+      <c r="S30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="S30" s="14" t="s">
+      <c r="T30" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="T30" s="14" t="s">
+      <c r="U30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="U30" s="14" t="s">
+      <c r="V30" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="V30" s="14" t="s">
+      <c r="W30" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q31" s="1" t="s">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R31" s="9" t="s">
+      <c r="S31" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S31" s="14" t="s">
+      <c r="T31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="T31" s="14" t="s">
+      <c r="U31" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="U31" s="14" t="s">
+      <c r="V31" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="V31" s="14" t="s">
+      <c r="W31" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q32" s="1" t="s">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R32" s="9" t="s">
+      <c r="S32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="S32" s="14" t="s">
+      <c r="T32" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="T32" s="14" t="s">
+      <c r="U32" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="U32" s="14" t="s">
+      <c r="V32" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="V32" s="14" t="s">
+      <c r="W32" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="17:22" x14ac:dyDescent="0.25">
-      <c r="Q33" s="1" t="s">
+    <row r="33" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R33" s="9" t="s">
+      <c r="S33" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="S33" s="14" t="s">
+      <c r="T33" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="T33" s="14" t="s">
+      <c r="U33" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="U33" s="14" t="s">
+      <c r="V33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="V33" s="14" t="s">
+      <c r="W33" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="17:22" x14ac:dyDescent="0.25">
-      <c r="Q34" s="1" t="s">
+    <row r="34" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R34" s="14" t="s">
+      <c r="S34" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="S34" s="14" t="s">
+      <c r="T34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="T34" s="14" t="s">
+      <c r="U34" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="U34" s="14" t="s">
+      <c r="V34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="V34" s="14" t="s">
+      <c r="W34" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="17:22" x14ac:dyDescent="0.25">
-      <c r="Q35" s="1" t="s">
+    <row r="35" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R35" s="14" t="s">
+      <c r="S35" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="S35" s="14" t="s">
+      <c r="T35" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="T35" s="14" t="s">
+      <c r="U35" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="U35" s="14" t="s">
+      <c r="V35" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="V35" s="14" t="s">
+      <c r="W35" s="14" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A19:G19"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="I19:O19"/>
+    <mergeCell ref="I10:P10"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="I19:P19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mapping program now shows neighbor matched grid num for predictions, and redid the code that matches accidents based on distance. Added new forecast files that only have one entry for a grid num for each dayframe, where previous versions would have more than one.
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DBC2CD-BE2C-4C34-8203-29C29AC5B5D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218D178D-810B-4982-AC81-BC3B3539EF3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main Numbers" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="55">
   <si>
     <t>TP</t>
   </si>
@@ -192,6 +193,12 @@
   </si>
   <si>
     <t>NTP</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>New (break)</t>
   </si>
 </sst>
 </file>
@@ -345,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -382,7 +389,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -392,12 +408,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -721,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD331EA-C281-4399-A27A-22CA50F1A7D5}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,15 +758,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
       <c r="I1" s="38" t="s">
         <v>51</v>
       </c>
@@ -1173,6 +1183,28 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I8" s="34"/>
+      <c r="J8" s="3">
+        <v>19.225806451612904</v>
+      </c>
+      <c r="K8" s="3">
+        <v>10.612903225806452</v>
+      </c>
+      <c r="L8" s="3">
+        <v>2370.8709677419356</v>
+      </c>
+      <c r="M8" s="3">
+        <v>155.29032258064515</v>
+      </c>
+      <c r="N8" s="2">
+        <v>67.576516113976979</v>
+      </c>
+      <c r="O8" s="2">
+        <v>93.855358184688683</v>
+      </c>
+      <c r="P8" s="3">
+        <v>14.064516129032258</v>
+      </c>
       <c r="R8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1193,6 +1225,14 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="35"/>
       <c r="R9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1213,24 +1253,24 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="I10" s="35" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="I10" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
       <c r="P10" s="37"/>
       <c r="R10" s="1" t="s">
         <v>16</v>
@@ -1678,25 +1718,25 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="I19" s="35" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="I19" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="37"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="42"/>
       <c r="R19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2314,4 +2354,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E095ABA1-36FB-4B15-9D2E-D02EAEE00886}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="15">
+        <v>28.451612903225808</v>
+      </c>
+      <c r="C3" s="15">
+        <v>34.161290322580648</v>
+      </c>
+      <c r="D3" s="15">
+        <v>4127.7419354838712</v>
+      </c>
+      <c r="E3" s="15">
+        <v>262.03225806451616</v>
+      </c>
+      <c r="F3" s="16">
+        <v>46.117155580882667</v>
+      </c>
+      <c r="G3" s="16">
+        <v>94.04732682027192</v>
+      </c>
+      <c r="H3" s="15">
+        <v>7.967741935483871</v>
+      </c>
+      <c r="I3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="3">
+        <v>19.225806451612904</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10.612903225806452</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2370.8709677419356</v>
+      </c>
+      <c r="E4" s="3">
+        <v>155.29032258064515</v>
+      </c>
+      <c r="F4" s="2">
+        <v>67.576516113976979</v>
+      </c>
+      <c r="G4" s="2">
+        <v>93.855358184688683</v>
+      </c>
+      <c r="H4" s="3">
+        <v>14.064516129032258</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2021 predictions redone, again. This time everything should be solid
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218D178D-810B-4982-AC81-BC3B3539EF3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D400114C-B476-432C-A74C-BEBCF0987780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Numbers" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Trimmed Version Break" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="53">
   <si>
     <t>TP</t>
   </si>
@@ -193,12 +193,6 @@
   </si>
   <si>
     <t>NTP</t>
-  </si>
-  <si>
-    <t>Old</t>
-  </si>
-  <si>
-    <t>New (break)</t>
   </si>
 </sst>
 </file>
@@ -732,7 +726,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:P8"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,46 +856,46 @@
         <v>6</v>
       </c>
       <c r="B3" s="15">
-        <v>20.483870967741936</v>
+        <v>10.225806451612904</v>
       </c>
       <c r="C3" s="15">
-        <v>42.12903225806452</v>
+        <v>25.967741935483872</v>
       </c>
       <c r="D3" s="15">
-        <v>4119.7741935483873</v>
+        <v>3505.4516129032259</v>
       </c>
       <c r="E3" s="15">
-        <v>270</v>
+        <v>207</v>
       </c>
       <c r="F3" s="16">
-        <v>32.967421219265887</v>
+        <v>28.394605845268121</v>
       </c>
       <c r="G3" s="16">
-        <v>93.866326112069842</v>
+        <v>94.434338001118618</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="15">
-        <v>28.451612903225808</v>
+        <v>16.774193548387096</v>
       </c>
       <c r="K3" s="15">
-        <v>34.161290322580648</v>
+        <v>20.225806451612904</v>
       </c>
       <c r="L3" s="15">
-        <v>4127.7419354838712</v>
+        <v>3511.1935483870966</v>
       </c>
       <c r="M3" s="15">
-        <v>262.03225806451616</v>
+        <v>200.45161290322579</v>
       </c>
       <c r="N3" s="16">
-        <v>46.117155580882667</v>
+        <v>45.216113534171448</v>
       </c>
       <c r="O3" s="16">
-        <v>94.04732682027192</v>
+        <v>94.609824342015003</v>
       </c>
       <c r="P3" s="15">
-        <v>7.967741935483871</v>
+        <v>12.096774193548388</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>9</v>
@@ -927,46 +921,46 @@
         <v>42</v>
       </c>
       <c r="B4" s="11">
-        <v>35.064516129032256</v>
+        <v>19.774193548387096</v>
       </c>
       <c r="C4" s="11">
-        <v>27.548387096774192</v>
+        <v>16.419354838709676</v>
       </c>
       <c r="D4" s="11">
-        <v>3686.7419354838707</v>
+        <v>3008.9032258064517</v>
       </c>
       <c r="E4" s="11">
-        <v>703.0322580645161</v>
+        <v>703.54838709677415</v>
       </c>
       <c r="F4" s="12">
-        <v>56.429834936558031</v>
+        <v>55.543546301714343</v>
       </c>
       <c r="G4" s="12">
-        <v>84.006794528998711</v>
+        <v>81.070131565702539</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="J4" s="11">
-        <v>49.483870967741936</v>
+        <v>27.70967741935484</v>
       </c>
       <c r="K4" s="11">
-        <v>13.129032258064516</v>
+        <v>10.387096774193548</v>
       </c>
       <c r="L4" s="11">
-        <v>3701.1612903225805</v>
+        <v>3014.9354838709678</v>
       </c>
       <c r="M4" s="11">
-        <v>688.61290322580646</v>
+        <v>695.61290322580646</v>
       </c>
       <c r="N4" s="12">
-        <v>80.149309072254894</v>
+        <v>72.982479671952007</v>
       </c>
       <c r="O4" s="12">
-        <v>84.335056504683791</v>
+        <v>81.274617168361345</v>
       </c>
       <c r="P4" s="11">
-        <v>14.419354838709678</v>
+        <v>21.258064516129032</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>10</v>
@@ -992,46 +986,46 @@
         <v>43</v>
       </c>
       <c r="B5" s="19">
-        <v>35</v>
+        <v>19.64516129032258</v>
       </c>
       <c r="C5" s="19">
-        <v>27.612903225806452</v>
+        <v>16.548387096774192</v>
       </c>
       <c r="D5" s="19">
-        <v>3696.2258064516127</v>
+        <v>3017.3870967741937</v>
       </c>
       <c r="E5" s="19">
-        <v>693.54838709677415</v>
+        <v>695.06451612903231</v>
       </c>
       <c r="F5" s="20">
-        <v>56.316638665548091</v>
+        <v>55.209727476740468</v>
       </c>
       <c r="G5" s="20">
-        <v>84.221882132102451</v>
+        <v>81.298249707799272</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J5" s="19">
-        <v>49.12903225806452</v>
+        <v>27.612903225806452</v>
       </c>
       <c r="K5" s="19">
-        <v>13.483870967741936</v>
+        <v>10.451612903225806</v>
       </c>
       <c r="L5" s="19">
-        <v>3710.3548387096776</v>
+        <v>3023.483870967742</v>
       </c>
       <c r="M5" s="19">
-        <v>679.41935483870964</v>
+        <v>687.09677419354841</v>
       </c>
       <c r="N5" s="20">
-        <v>79.528640881418781</v>
+        <v>72.686222842529631</v>
       </c>
       <c r="O5" s="20">
-        <v>84.543564737159983</v>
+        <v>81.50415464838504</v>
       </c>
       <c r="P5" s="19">
-        <v>14.129032258064516</v>
+        <v>21.322580645161292</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>11</v>
@@ -1057,46 +1051,46 @@
         <v>44</v>
       </c>
       <c r="B6" s="22">
-        <v>21.451612903225808</v>
+        <v>12.32258064516129</v>
       </c>
       <c r="C6" s="22">
-        <v>41.161290322580648</v>
+        <v>23.870967741935484</v>
       </c>
       <c r="D6" s="22">
-        <v>4103.2258064516127</v>
+        <v>3428.2580645161293</v>
       </c>
       <c r="E6" s="22">
-        <v>286.54838709677421</v>
+        <v>284.19354838709677</v>
       </c>
       <c r="F6" s="23">
-        <v>34.091820100119499</v>
+        <v>34.654998672999255</v>
       </c>
       <c r="G6" s="23">
-        <v>93.481193786837395</v>
+        <v>92.353552846481151</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>44</v>
       </c>
       <c r="J6" s="22">
-        <v>29.387096774193548</v>
+        <v>19.903225806451612</v>
       </c>
       <c r="K6" s="22">
-        <v>33.225806451612904</v>
+        <v>17.483870967741936</v>
       </c>
       <c r="L6" s="22">
-        <v>4111.1612903225805</v>
+        <v>3434.6451612903224</v>
       </c>
       <c r="M6" s="22">
-        <v>278.61290322580646</v>
+        <v>276.61290322580646</v>
       </c>
       <c r="N6" s="23">
-        <v>47.182106813471258</v>
+        <v>53.389855688626454</v>
       </c>
       <c r="O6" s="23">
-        <v>93.661473513021477</v>
+        <v>92.555727815915532</v>
       </c>
       <c r="P6" s="22">
-        <v>7.935483870967742</v>
+        <v>14.870967741935484</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>12</v>
@@ -1122,46 +1116,46 @@
         <v>45</v>
       </c>
       <c r="B7" s="27">
-        <v>36.258064516129032</v>
+        <v>20.516129032258064</v>
       </c>
       <c r="C7" s="27">
-        <v>26.35483870967742</v>
+        <v>15.67741935483871</v>
       </c>
       <c r="D7" s="27">
-        <v>3666.2903225806454</v>
+        <v>3016.3870967741937</v>
       </c>
       <c r="E7" s="27">
-        <v>723.48387096774195</v>
+        <v>696.06451612903231</v>
       </c>
       <c r="F7" s="28">
-        <v>58.108574742803064</v>
+        <v>57.252212298330448</v>
       </c>
       <c r="G7" s="28">
-        <v>83.542654648323293</v>
+        <v>81.273665169741491</v>
       </c>
       <c r="I7" s="26" t="s">
         <v>45</v>
       </c>
       <c r="J7" s="27">
-        <v>50.645161290322584</v>
+        <v>27.93548387096774</v>
       </c>
       <c r="K7" s="27">
-        <v>11.96774193548387</v>
+        <v>10.225806451612904</v>
       </c>
       <c r="L7" s="27">
-        <v>3680.6774193548385</v>
+        <v>3021.8387096774195</v>
       </c>
       <c r="M7" s="27">
-        <v>709.09677419354841</v>
+        <v>688.64516129032256</v>
       </c>
       <c r="N7" s="28">
-        <v>81.452345269896909</v>
+        <v>73.635726504274146</v>
       </c>
       <c r="O7" s="28">
-        <v>83.869996830115056</v>
+        <v>81.464069327952075</v>
       </c>
       <c r="P7" s="27">
-        <v>14.387096774193548</v>
+        <v>20.838709677419356</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>13</v>
@@ -1184,27 +1178,6 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I8" s="34"/>
-      <c r="J8" s="3">
-        <v>19.225806451612904</v>
-      </c>
-      <c r="K8" s="3">
-        <v>10.612903225806452</v>
-      </c>
-      <c r="L8" s="3">
-        <v>2370.8709677419356</v>
-      </c>
-      <c r="M8" s="3">
-        <v>155.29032258064515</v>
-      </c>
-      <c r="N8" s="2">
-        <v>67.576516113976979</v>
-      </c>
-      <c r="O8" s="2">
-        <v>93.855358184688683</v>
-      </c>
-      <c r="P8" s="3">
-        <v>14.064516129032258</v>
-      </c>
       <c r="R8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1357,46 +1330,46 @@
         <v>6</v>
       </c>
       <c r="B12" s="31">
-        <v>8.3548387096774199</v>
+        <v>4.354838709677419</v>
       </c>
       <c r="C12" s="31">
-        <v>54.258064516129032</v>
+        <v>31.838709677419356</v>
       </c>
       <c r="D12" s="31">
-        <v>4306.322580645161</v>
+        <v>3649.5806451612902</v>
       </c>
       <c r="E12" s="31">
-        <v>83.451612903225808</v>
+        <v>62.87096774193548</v>
       </c>
       <c r="F12" s="32">
-        <v>10.086283732417924</v>
+        <v>8.9383886725521187</v>
       </c>
       <c r="G12" s="32">
-        <v>91.715479750131749</v>
+        <v>91.901288300393915</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J12" s="31">
-        <v>11.870967741935484</v>
+        <v>8.7096774193548381</v>
       </c>
       <c r="K12" s="31">
-        <v>50.741935483870968</v>
+        <v>27.70967741935484</v>
       </c>
       <c r="L12" s="31">
-        <v>4309.8387096774195</v>
+        <v>3653.7096774193546</v>
       </c>
       <c r="M12" s="31">
-        <v>79.935483870967744</v>
+        <v>58.516129032258064</v>
       </c>
       <c r="N12" s="32">
-        <v>15.913783677093578</v>
+        <v>24.007018768494138</v>
       </c>
       <c r="O12" s="32">
-        <v>91.795223056364762</v>
+        <v>98.426885765401224</v>
       </c>
       <c r="P12" s="15">
-        <v>3.5161290322580645</v>
+        <v>6.32258064516129</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>18</v>
@@ -1422,46 +1395,46 @@
         <v>42</v>
       </c>
       <c r="B13" s="11">
-        <v>19.870967741935484</v>
+        <v>11.774193548387096</v>
       </c>
       <c r="C13" s="11">
-        <v>42.741935483870968</v>
+        <v>24.419354838709676</v>
       </c>
       <c r="D13" s="11">
-        <v>4150.9677419354839</v>
+        <v>3466.8387096774195</v>
       </c>
       <c r="E13" s="11">
-        <v>238.80645161290323</v>
+        <v>245.61290322580646</v>
       </c>
       <c r="F13" s="12">
-        <v>31.432146871392032</v>
+        <v>32.835750501736982</v>
       </c>
       <c r="G13" s="12">
-        <v>94.566913986806313</v>
+        <v>93.391215441944198</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="11">
-        <v>27.64516129032258</v>
+        <v>19.06451612903226</v>
       </c>
       <c r="K13" s="11">
-        <v>34.967741935483872</v>
+        <v>18.193548387096776</v>
       </c>
       <c r="L13" s="11">
-        <v>4158.7419354838712</v>
+        <v>3473.0645161290322</v>
       </c>
       <c r="M13" s="11">
-        <v>231.03225806451613</v>
+        <v>238.32258064516128</v>
       </c>
       <c r="N13" s="12">
-        <v>44.313172788593675</v>
+        <v>51.436775848645432</v>
       </c>
       <c r="O13" s="12">
-        <v>94.743640199565377</v>
+        <v>93.58625430624798</v>
       </c>
       <c r="P13" s="11">
-        <v>7.774193548387097</v>
+        <v>14.193548387096774</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>19</v>
@@ -1487,46 +1460,46 @@
         <v>43</v>
       </c>
       <c r="B14" s="19">
-        <v>19.774193548387096</v>
+        <v>11.838709677419354</v>
       </c>
       <c r="C14" s="19">
-        <v>42.838709677419352</v>
+        <v>24.35483870967742</v>
       </c>
       <c r="D14" s="19">
-        <v>4153.6129032258068</v>
+        <v>3469.516129032258</v>
       </c>
       <c r="E14" s="19">
-        <v>236.16129032258064</v>
+        <v>242.93548387096774</v>
       </c>
       <c r="F14" s="20">
-        <v>31.286727909479879</v>
+        <v>33.029636081145767</v>
       </c>
       <c r="G14" s="20">
-        <v>94.626760916422313</v>
+        <v>93.46293190264997</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="19">
-        <v>27.516129032258064</v>
+        <v>19.161290322580644</v>
       </c>
       <c r="K14" s="19">
-        <v>35.096774193548384</v>
+        <v>18.096774193548388</v>
       </c>
       <c r="L14" s="19">
-        <v>4161.3548387096771</v>
+        <v>3475.7741935483873</v>
       </c>
       <c r="M14" s="19">
-        <v>228.41935483870967</v>
+        <v>235.61290322580646</v>
       </c>
       <c r="N14" s="20">
-        <v>44.131911532774708</v>
+        <v>51.703626097793091</v>
       </c>
       <c r="O14" s="20">
-        <v>94.802753674846414</v>
+        <v>93.658861330230692</v>
       </c>
       <c r="P14" s="19">
-        <v>7.741935483870968</v>
+        <v>14.35483870967742</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>20</v>
@@ -1552,46 +1525,46 @@
         <v>44</v>
       </c>
       <c r="B15" s="22">
-        <v>10.741935483870968</v>
+        <v>6.258064516129032</v>
       </c>
       <c r="C15" s="22">
-        <v>51.87096774193548</v>
+        <v>29.93548387096774</v>
       </c>
       <c r="D15" s="22">
-        <v>4291.4516129032254</v>
+        <v>3613.2903225806454</v>
       </c>
       <c r="E15" s="22">
-        <v>98.322580645161295</v>
+        <v>99.161290322580641</v>
       </c>
       <c r="F15" s="23">
-        <v>17.009450859865115</v>
+        <v>17.6395826584946</v>
       </c>
       <c r="G15" s="23">
-        <v>97.762639665280531</v>
+        <v>97.331805347047336</v>
       </c>
       <c r="I15" s="25" t="s">
         <v>44</v>
       </c>
       <c r="J15" s="22">
-        <v>14.709677419354838</v>
+        <v>12.161290322580646</v>
       </c>
       <c r="K15" s="22">
-        <v>47.903225806451616</v>
+        <v>24.483870967741936</v>
       </c>
       <c r="L15" s="22">
-        <v>4295.4193548387093</v>
+        <v>3618.7419354838707</v>
       </c>
       <c r="M15" s="22">
-        <v>94.354838709677423</v>
+        <v>93.258064516129039</v>
       </c>
       <c r="N15" s="23">
-        <v>23.410546202487399</v>
+        <v>33.050914180104179</v>
       </c>
       <c r="O15" s="23">
-        <v>97.852913170256514</v>
+        <v>97.490727445193983</v>
       </c>
       <c r="P15" s="22">
-        <v>3.967741935483871</v>
+        <v>8.741935483870968</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>21</v>
@@ -1617,46 +1590,46 @@
         <v>45</v>
       </c>
       <c r="B16" s="27">
-        <v>18.903225806451612</v>
+        <v>11</v>
       </c>
       <c r="C16" s="27">
-        <v>43.70967741935484</v>
+        <v>25.193548387096776</v>
       </c>
       <c r="D16" s="27">
-        <v>4173.1935483870966</v>
+        <v>3496.6774193548385</v>
       </c>
       <c r="E16" s="27">
-        <v>216.58064516129033</v>
+        <v>215.7741935483871</v>
       </c>
       <c r="F16" s="28">
-        <v>30.006507510804845</v>
+        <v>30.674767780735042</v>
       </c>
       <c r="G16" s="28">
-        <v>95.071603315232068</v>
+        <v>94.193115057393456</v>
       </c>
       <c r="I16" s="26" t="s">
         <v>45</v>
       </c>
       <c r="J16" s="27">
-        <v>25.548387096774192</v>
+        <v>18.096774193548388</v>
       </c>
       <c r="K16" s="27">
-        <v>37.064516129032256</v>
+        <v>19</v>
       </c>
       <c r="L16" s="27">
-        <v>4179.8387096774195</v>
+        <v>3502.8709677419356</v>
       </c>
       <c r="M16" s="27">
-        <v>209.93548387096774</v>
+        <v>208.67741935483872</v>
       </c>
       <c r="N16" s="28">
-        <v>40.892388432441187</v>
+        <v>48.694675566650446</v>
       </c>
       <c r="O16" s="28">
-        <v>95.222632512794803</v>
+        <v>94.383423843573766</v>
       </c>
       <c r="P16" s="27">
-        <v>6.645161290322581</v>
+        <v>13.419354838709678</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>22</v>
@@ -1822,46 +1795,46 @@
         <v>6</v>
       </c>
       <c r="B21" s="31">
-        <v>15.193548387096774</v>
+        <v>7.612903225806452</v>
       </c>
       <c r="C21" s="31">
-        <v>47.41935483870968</v>
+        <v>28.580645161290324</v>
       </c>
       <c r="D21" s="31">
-        <v>4216.1290322580644</v>
+        <v>3578.9677419354839</v>
       </c>
       <c r="E21" s="31">
-        <v>173.64516129032259</v>
+        <v>133.48387096774192</v>
       </c>
       <c r="F21" s="32">
-        <v>24.369636715007047</v>
+        <v>21.162550990811138</v>
       </c>
       <c r="G21" s="32">
-        <v>96.055115466237112</v>
+        <v>96.410655344079004</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J21" s="31">
-        <v>21.193548387096776</v>
+        <v>13.709677419354838</v>
       </c>
       <c r="K21" s="31">
-        <v>41.41935483870968</v>
+        <v>23.096774193548388</v>
       </c>
       <c r="L21" s="31">
-        <v>4222.1290322580644</v>
+        <v>3584.4516129032259</v>
       </c>
       <c r="M21" s="31">
-        <v>167.64516129032259</v>
+        <v>127.38709677419355</v>
       </c>
       <c r="N21" s="32">
-        <v>34.433244066226969</v>
+        <v>37.128836589552456</v>
       </c>
       <c r="O21" s="32">
-        <v>96.19144771472719</v>
+        <v>96.574400226107613</v>
       </c>
       <c r="P21" s="31">
-        <v>6</v>
+        <v>9.8387096774193541</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>27</v>
@@ -1887,46 +1860,46 @@
         <v>42</v>
       </c>
       <c r="B22" s="11">
-        <v>29.806451612903224</v>
+        <v>16.548387096774192</v>
       </c>
       <c r="C22" s="11">
-        <v>32.806451612903224</v>
+        <v>19.64516129032258</v>
       </c>
       <c r="D22" s="11">
-        <v>3925.8709677419356</v>
+        <v>3238.6129032258063</v>
       </c>
       <c r="E22" s="11">
-        <v>463.90322580645159</v>
+        <v>473.83870967741933</v>
       </c>
       <c r="F22" s="12">
-        <v>47.867886696854754</v>
+        <v>46.554460726975762</v>
       </c>
       <c r="G22" s="12">
-        <v>89.445897020202395</v>
+        <v>87.250509849082576</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>42</v>
       </c>
       <c r="J22" s="11">
-        <v>41</v>
+        <v>24.677419354838708</v>
       </c>
       <c r="K22" s="11">
-        <v>21.612903225806452</v>
+        <v>13</v>
       </c>
       <c r="L22" s="11">
-        <v>3937.0645161290322</v>
+        <v>3245.2580645161293</v>
       </c>
       <c r="M22" s="11">
-        <v>452.70967741935482</v>
+        <v>465.70967741935482</v>
       </c>
       <c r="N22" s="12">
-        <v>66.1974474462789</v>
+        <v>65.633404193846658</v>
       </c>
       <c r="O22" s="12">
-        <v>89.700721360683744</v>
+        <v>87.465755427354523</v>
       </c>
       <c r="P22" s="11">
-        <v>11.193548387096774</v>
+        <v>18.677419354838708</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>28</v>
@@ -1952,46 +1925,46 @@
         <v>43</v>
       </c>
       <c r="B23" s="19">
-        <v>29.677419354838708</v>
+        <v>16.612903225806452</v>
       </c>
       <c r="C23" s="19">
-        <v>32.935483870967744</v>
+        <v>19.580645161290324</v>
       </c>
       <c r="D23" s="19">
-        <v>3933.2258064516127</v>
+        <v>3244.6129032258063</v>
       </c>
       <c r="E23" s="19">
-        <v>456.54838709677421</v>
+        <v>467.83870967741933</v>
       </c>
       <c r="F23" s="20">
-        <v>47.643872512761895</v>
+        <v>46.691444381839652</v>
       </c>
       <c r="G23" s="20">
-        <v>89.612897925432904</v>
+        <v>87.411997543954925</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>43</v>
       </c>
       <c r="J23" s="19">
-        <v>40.967741935483872</v>
+        <v>24.741935483870968</v>
       </c>
       <c r="K23" s="19">
-        <v>21.64516129032258</v>
+        <v>12.935483870967742</v>
       </c>
       <c r="L23" s="19">
-        <v>3944.516129032258</v>
+        <v>3251.2580645161293</v>
       </c>
       <c r="M23" s="19">
-        <v>445.25806451612902</v>
+        <v>459.70967741935482</v>
       </c>
       <c r="N23" s="20">
-        <v>66.157139063244443</v>
+        <v>65.757261762050973</v>
       </c>
       <c r="O23" s="20">
-        <v>89.869914418749701</v>
+        <v>87.627330580965008</v>
       </c>
       <c r="P23" s="19">
-        <v>11.290322580645162</v>
+        <v>18.64516129032258</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>29</v>
@@ -2017,46 +1990,46 @@
         <v>44</v>
       </c>
       <c r="B24" s="22">
-        <v>17.032258064516128</v>
+        <v>10</v>
       </c>
       <c r="C24" s="22">
-        <v>45.58064516129032</v>
+        <v>26.193548387096776</v>
       </c>
       <c r="D24" s="22">
-        <v>4199.1935483870966</v>
+        <v>3521.8709677419356</v>
       </c>
       <c r="E24" s="22">
         <v>190.58064516129033</v>
       </c>
       <c r="F24" s="23">
-        <v>27.121949823522591</v>
+        <v>27.928619096123331</v>
       </c>
       <c r="G24" s="23">
-        <v>95.66381849693002</v>
+        <v>94.871803911349772</v>
       </c>
       <c r="I24" s="25" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="22">
-        <v>23.06451612903226</v>
+        <v>16.806451612903224</v>
       </c>
       <c r="K24" s="22">
-        <v>39.548387096774192</v>
+        <v>20.29032258064516</v>
       </c>
       <c r="L24" s="22">
-        <v>4205.2258064516127</v>
+        <v>3527.7741935483873</v>
       </c>
       <c r="M24" s="22">
-        <v>184.54838709677421</v>
+        <v>183.7741935483871</v>
       </c>
       <c r="N24" s="23">
-        <v>37.01474743980296</v>
+        <v>45.348520251432696</v>
       </c>
       <c r="O24" s="23">
-        <v>95.800937942331601</v>
+        <v>95.054464319773032</v>
       </c>
       <c r="P24" s="22">
-        <v>6.032258064516129</v>
+        <v>12.741935483870968</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>30</v>
@@ -2082,46 +2055,46 @@
         <v>45</v>
       </c>
       <c r="B25" s="27">
-        <v>28.903225806451612</v>
+        <v>15.96774193548387</v>
       </c>
       <c r="C25" s="27">
-        <v>33.70967741935484</v>
+        <v>20.225806451612904</v>
       </c>
       <c r="D25" s="27">
-        <v>3947.516129032258</v>
+        <v>3276.516129032258</v>
       </c>
       <c r="E25" s="27">
-        <v>442.25806451612902</v>
+        <v>435.93548387096774</v>
       </c>
       <c r="F25" s="28">
-        <v>46.313100591954786</v>
+        <v>44.656254027235477</v>
       </c>
       <c r="G25" s="28">
-        <v>89.937514605778802</v>
+        <v>88.269633472672425</v>
       </c>
       <c r="I25" s="26" t="s">
         <v>45</v>
       </c>
       <c r="J25" s="27">
-        <v>39.87096774193548</v>
+        <v>24.096774193548388</v>
       </c>
       <c r="K25" s="27">
-        <v>22.741935483870968</v>
+        <v>13.67741935483871</v>
       </c>
       <c r="L25" s="27">
-        <v>3958.483870967742</v>
+        <v>3283.0645161290322</v>
       </c>
       <c r="M25" s="27">
-        <v>431.29032258064518</v>
+        <v>427.80645161290323</v>
       </c>
       <c r="N25" s="28">
-        <v>64.30291994486133</v>
+        <v>63.981506864719215</v>
       </c>
       <c r="O25" s="28">
-        <v>90.186976579405197</v>
+        <v>88.484743038878236</v>
       </c>
       <c r="P25" s="27">
-        <v>10.96774193548387</v>
+        <v>18.193548387096776</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>31</v>
@@ -2357,39 +2330,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E095ABA1-36FB-4B15-9D2E-D02EAEE00886}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EEF8CF-29A3-49DF-A898-012230C01B0E}">
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="3"/>
+    <col min="18" max="23" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="I1" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="R1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -2409,69 +2418,1519 @@
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="33" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="15">
-        <v>28.451612903225808</v>
+        <v>9.7096774193548381</v>
       </c>
       <c r="C3" s="15">
-        <v>34.161290322580648</v>
+        <v>26.483870967741936</v>
       </c>
       <c r="D3" s="15">
-        <v>4127.7419354838712</v>
+        <v>1997.2258064516129</v>
       </c>
       <c r="E3" s="15">
-        <v>262.03225806451616</v>
+        <v>118.58064516129032</v>
       </c>
       <c r="F3" s="16">
-        <v>46.117155580882667</v>
+        <v>27.023364415296825</v>
       </c>
       <c r="G3" s="16">
-        <v>94.04732682027192</v>
-      </c>
-      <c r="H3" s="15">
-        <v>7.967741935483871</v>
-      </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="3">
-        <v>19.225806451612904</v>
-      </c>
-      <c r="C4" s="3">
-        <v>10.612903225806452</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2370.8709677419356</v>
-      </c>
-      <c r="E4" s="3">
-        <v>155.29032258064515</v>
-      </c>
-      <c r="F4" s="2">
-        <v>67.576516113976979</v>
-      </c>
-      <c r="G4" s="2">
-        <v>93.855358184688683</v>
-      </c>
-      <c r="H4" s="3">
-        <v>14.064516129032258</v>
-      </c>
-      <c r="I4" t="s">
-        <v>54</v>
+        <v>94.395725819075665</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="15">
+        <v>16.870967741935484</v>
+      </c>
+      <c r="K3" s="15">
+        <v>20.129032258064516</v>
+      </c>
+      <c r="L3" s="15">
+        <v>2003.5806451612902</v>
+      </c>
+      <c r="M3" s="15">
+        <v>111.41935483870968</v>
+      </c>
+      <c r="N3" s="16">
+        <v>45.410334998134033</v>
+      </c>
+      <c r="O3" s="16">
+        <v>94.731944746599197</v>
+      </c>
+      <c r="P3" s="15">
+        <v>12.548387096774194</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="W3" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="11">
+        <v>19.70967741935484</v>
+      </c>
+      <c r="C4" s="11">
+        <v>16.483870967741936</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1705.3870967741937</v>
+      </c>
+      <c r="E4" s="11">
+        <v>410.41935483870969</v>
+      </c>
+      <c r="F4" s="12">
+        <v>55.438539822247101</v>
+      </c>
+      <c r="G4" s="12">
+        <v>80.608223925308465</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="11">
+        <v>27.93548387096774</v>
+      </c>
+      <c r="K4" s="11">
+        <v>10.096774193548388</v>
+      </c>
+      <c r="L4" s="11">
+        <v>1711.7741935483871</v>
+      </c>
+      <c r="M4" s="11">
+        <v>402.19354838709677</v>
+      </c>
+      <c r="N4" s="12">
+        <v>73.612960840263938</v>
+      </c>
+      <c r="O4" s="12">
+        <v>80.980068928827649</v>
+      </c>
+      <c r="P4" s="11">
+        <v>21.419354838709676</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="W4" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="19">
+        <v>19.483870967741936</v>
+      </c>
+      <c r="C5" s="19">
+        <v>16.70967741935484</v>
+      </c>
+      <c r="D5" s="19">
+        <v>1712.0645161290322</v>
+      </c>
+      <c r="E5" s="19">
+        <v>403.74193548387098</v>
+      </c>
+      <c r="F5" s="20">
+        <v>54.858279720147451</v>
+      </c>
+      <c r="G5" s="20">
+        <v>80.923078798604422</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="19">
+        <v>27.903225806451612</v>
+      </c>
+      <c r="K5" s="19">
+        <v>10.161290322580646</v>
+      </c>
+      <c r="L5" s="19">
+        <v>1718.6129032258063</v>
+      </c>
+      <c r="M5" s="19">
+        <v>395.32258064516128</v>
+      </c>
+      <c r="N5" s="20">
+        <v>73.445030421858476</v>
+      </c>
+      <c r="O5" s="20">
+        <v>81.304128123370347</v>
+      </c>
+      <c r="P5" s="19">
+        <v>21.516129032258064</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="V5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="22">
+        <v>12.258064516129032</v>
+      </c>
+      <c r="C6" s="22">
+        <v>23.93548387096774</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1952.2903225806451</v>
+      </c>
+      <c r="E6" s="22">
+        <v>163.51612903225808</v>
+      </c>
+      <c r="F6" s="23">
+        <v>34.487652040286136</v>
+      </c>
+      <c r="G6" s="23">
+        <v>92.273579471996612</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="22">
+        <v>19.903225806451612</v>
+      </c>
+      <c r="K6" s="22">
+        <v>17.451612903225808</v>
+      </c>
+      <c r="L6" s="22">
+        <v>1958.7741935483871</v>
+      </c>
+      <c r="M6" s="22">
+        <v>155.87096774193549</v>
+      </c>
+      <c r="N6" s="23">
+        <v>53.152763520952796</v>
+      </c>
+      <c r="O6" s="23">
+        <v>92.630706813638369</v>
+      </c>
+      <c r="P6" s="22">
+        <v>14.64516129032258</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="27">
+        <v>20.322580645161292</v>
+      </c>
+      <c r="C7" s="27">
+        <v>15.870967741935484</v>
+      </c>
+      <c r="D7" s="27">
+        <v>1709.8064516129032</v>
+      </c>
+      <c r="E7" s="27">
+        <v>406</v>
+      </c>
+      <c r="F7" s="28">
+        <v>56.883689482876164</v>
+      </c>
+      <c r="G7" s="28">
+        <v>80.817253985149662</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="27">
+        <v>28.129032258064516</v>
+      </c>
+      <c r="K7" s="27">
+        <v>10</v>
+      </c>
+      <c r="L7" s="27">
+        <v>1715.6774193548388</v>
+      </c>
+      <c r="M7" s="27">
+        <v>398.19354838709677</v>
+      </c>
+      <c r="N7" s="28">
+        <v>74.19537989673411</v>
+      </c>
+      <c r="O7" s="28">
+        <v>81.168358362598084</v>
+      </c>
+      <c r="P7" s="27">
+        <v>21.06451612903226</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="V7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="W7" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I8" s="34"/>
+      <c r="R8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="T8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="V8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="35"/>
+      <c r="R9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="U9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="I10" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="R10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="V10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="W10" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="V11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="W11" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="31">
+        <v>4.354838709677419</v>
+      </c>
+      <c r="C12" s="31">
+        <v>31.838709677419356</v>
+      </c>
+      <c r="D12" s="31">
+        <v>2079.0645161290322</v>
+      </c>
+      <c r="E12" s="31">
+        <v>36.741935483870968</v>
+      </c>
+      <c r="F12" s="32">
+        <v>8.9352893471059964</v>
+      </c>
+      <c r="G12" s="32">
+        <v>91.863216652372046</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="31">
+        <v>8.5161290322580641</v>
+      </c>
+      <c r="K12" s="31">
+        <v>27.870967741935484</v>
+      </c>
+      <c r="L12" s="31">
+        <v>2083.0322580645161</v>
+      </c>
+      <c r="M12" s="31">
+        <v>32.58064516129032</v>
+      </c>
+      <c r="N12" s="32">
+        <v>23.550713713848147</v>
+      </c>
+      <c r="O12" s="32">
+        <v>98.460109149759759</v>
+      </c>
+      <c r="P12" s="15">
+        <v>5.903225806451613</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="U12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="V12" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="W12" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="11">
+        <v>11.548387096774194</v>
+      </c>
+      <c r="C13" s="11">
+        <v>24.64516129032258</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1975.3225806451612</v>
+      </c>
+      <c r="E13" s="11">
+        <v>140.48387096774192</v>
+      </c>
+      <c r="F13" s="12">
+        <v>32.215534718256301</v>
+      </c>
+      <c r="G13" s="12">
+        <v>93.362066071612887</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="11">
+        <v>19</v>
+      </c>
+      <c r="K13" s="11">
+        <v>18.258064516129032</v>
+      </c>
+      <c r="L13" s="11">
+        <v>1981.7096774193549</v>
+      </c>
+      <c r="M13" s="11">
+        <v>133.03225806451613</v>
+      </c>
+      <c r="N13" s="12">
+        <v>51.240972713379612</v>
+      </c>
+      <c r="O13" s="12">
+        <v>93.7108860655119</v>
+      </c>
+      <c r="P13" s="11">
+        <v>14.096774193548388</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="V13" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="W13" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="19">
+        <v>11.483870967741936</v>
+      </c>
+      <c r="C14" s="19">
+        <v>24.70967741935484</v>
+      </c>
+      <c r="D14" s="19">
+        <v>1977.0967741935483</v>
+      </c>
+      <c r="E14" s="19">
+        <v>138.70967741935485</v>
+      </c>
+      <c r="F14" s="20">
+        <v>32.070926055268039</v>
+      </c>
+      <c r="G14" s="20">
+        <v>93.445678770006396</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="19">
+        <v>18.838709677419356</v>
+      </c>
+      <c r="K14" s="19">
+        <v>18.387096774193548</v>
+      </c>
+      <c r="L14" s="19">
+        <v>1983.4193548387098</v>
+      </c>
+      <c r="M14" s="19">
+        <v>131.35483870967741</v>
+      </c>
+      <c r="N14" s="20">
+        <v>50.822862410619365</v>
+      </c>
+      <c r="O14" s="20">
+        <v>93.790044210109016</v>
+      </c>
+      <c r="P14" s="19">
+        <v>14.03225806451613</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="V14" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="22">
+        <v>6.419354838709677</v>
+      </c>
+      <c r="C15" s="22">
+        <v>29.774193548387096</v>
+      </c>
+      <c r="D15" s="22">
+        <v>2060.6129032258063</v>
+      </c>
+      <c r="E15" s="22">
+        <v>55.193548387096776</v>
+      </c>
+      <c r="F15" s="23">
+        <v>17.966334389030983</v>
+      </c>
+      <c r="G15" s="23">
+        <v>97.392144258964748</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="22">
+        <v>11.903225806451612</v>
+      </c>
+      <c r="K15" s="22">
+        <v>24.741935483870968</v>
+      </c>
+      <c r="L15" s="22">
+        <v>2065.6451612903224</v>
+      </c>
+      <c r="M15" s="22">
+        <v>49.70967741935484</v>
+      </c>
+      <c r="N15" s="23">
+        <v>32.286908896686533</v>
+      </c>
+      <c r="O15" s="23">
+        <v>97.651051751538915</v>
+      </c>
+      <c r="P15" s="22">
+        <v>8.4516129032258061</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="U15" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="V15" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="W15" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="27">
+        <v>10.903225806451612</v>
+      </c>
+      <c r="C16" s="27">
+        <v>25.29032258064516</v>
+      </c>
+      <c r="D16" s="27">
+        <v>1995.1290322580646</v>
+      </c>
+      <c r="E16" s="27">
+        <v>120.6774193548387</v>
+      </c>
+      <c r="F16" s="28">
+        <v>30.489656145462614</v>
+      </c>
+      <c r="G16" s="28">
+        <v>94.297674072261827</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="27">
+        <v>18.258064516129032</v>
+      </c>
+      <c r="K16" s="27">
+        <v>18.838709677419356</v>
+      </c>
+      <c r="L16" s="27">
+        <v>2001.5806451612902</v>
+      </c>
+      <c r="M16" s="27">
+        <v>113.3225806451613</v>
+      </c>
+      <c r="N16" s="28">
+        <v>49.083180744084167</v>
+      </c>
+      <c r="O16" s="28">
+        <v>94.643148750587514</v>
+      </c>
+      <c r="P16" s="27">
+        <v>13.193548387096774</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="V16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="V17" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="T18" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="U18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V18" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="I19" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="42"/>
+      <c r="R19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="U19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="W19" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="U20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="W20" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="31">
+        <v>7.612903225806452</v>
+      </c>
+      <c r="C21" s="31">
+        <v>28.580645161290324</v>
+      </c>
+      <c r="D21" s="31">
+        <v>2039.2903225806451</v>
+      </c>
+      <c r="E21" s="31">
+        <v>76.516129032258064</v>
+      </c>
+      <c r="F21" s="32">
+        <v>21.075926441629722</v>
+      </c>
+      <c r="G21" s="32">
+        <v>96.383846550095058</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="31">
+        <v>14</v>
+      </c>
+      <c r="K21" s="31">
+        <v>22.774193548387096</v>
+      </c>
+      <c r="L21" s="31">
+        <v>2045.0967741935483</v>
+      </c>
+      <c r="M21" s="31">
+        <v>70.129032258064512</v>
+      </c>
+      <c r="N21" s="32">
+        <v>37.624871165204048</v>
+      </c>
+      <c r="O21" s="32">
+        <v>96.684872982573182</v>
+      </c>
+      <c r="P21" s="31">
+        <v>9.9677419354838701</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="V21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="11">
+        <v>16.548387096774192</v>
+      </c>
+      <c r="C22" s="11">
+        <v>19.64516129032258</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1840.2258064516129</v>
+      </c>
+      <c r="E22" s="11">
+        <v>275.58064516129031</v>
+      </c>
+      <c r="F22" s="12">
+        <v>46.75935682834389</v>
+      </c>
+      <c r="G22" s="12">
+        <v>86.97838597003792</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="11">
+        <v>24.870967741935484</v>
+      </c>
+      <c r="K22" s="11">
+        <v>12.838709677419354</v>
+      </c>
+      <c r="L22" s="11">
+        <v>1847.0322580645161</v>
+      </c>
+      <c r="M22" s="11">
+        <v>267.25806451612902</v>
+      </c>
+      <c r="N22" s="12">
+        <v>66.259053201450683</v>
+      </c>
+      <c r="O22" s="12">
+        <v>87.362220080812577</v>
+      </c>
+      <c r="P22" s="11">
+        <v>18.741935483870968</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="U22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="W22" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="19">
+        <v>16.35483870967742</v>
+      </c>
+      <c r="C23" s="19">
+        <v>19.838709677419356</v>
+      </c>
+      <c r="D23" s="19">
+        <v>1845.0322580645161</v>
+      </c>
+      <c r="E23" s="19">
+        <v>270.77419354838707</v>
+      </c>
+      <c r="F23" s="20">
+        <v>46.185046934774029</v>
+      </c>
+      <c r="G23" s="20">
+        <v>87.205257283800989</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="19">
+        <v>24.741935483870968</v>
+      </c>
+      <c r="K23" s="19">
+        <v>12.96774193548387</v>
+      </c>
+      <c r="L23" s="19">
+        <v>1851.9032258064517</v>
+      </c>
+      <c r="M23" s="19">
+        <v>262.38709677419354</v>
+      </c>
+      <c r="N23" s="20">
+        <v>65.884509941633894</v>
+      </c>
+      <c r="O23" s="20">
+        <v>87.592342042585571</v>
+      </c>
+      <c r="P23" s="19">
+        <v>18.64516129032258</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="U23" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="W23" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="22">
+        <v>9.7096774193548381</v>
+      </c>
+      <c r="C24" s="22">
+        <v>26.483870967741936</v>
+      </c>
+      <c r="D24" s="22">
+        <v>2007.8709677419354</v>
+      </c>
+      <c r="E24" s="22">
+        <v>107.93548387096774</v>
+      </c>
+      <c r="F24" s="23">
+        <v>26.996374015768939</v>
+      </c>
+      <c r="G24" s="23">
+        <v>94.899937794875171</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="22">
+        <v>16.903225806451612</v>
+      </c>
+      <c r="K24" s="22">
+        <v>20.161290322580644</v>
+      </c>
+      <c r="L24" s="22">
+        <v>2014.1935483870968</v>
+      </c>
+      <c r="M24" s="22">
+        <v>100.74193548387096</v>
+      </c>
+      <c r="N24" s="23">
+        <v>45.453955508217774</v>
+      </c>
+      <c r="O24" s="23">
+        <v>95.238008554386155</v>
+      </c>
+      <c r="P24" s="22">
+        <v>12.64516129032258</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="U24" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="V24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W24" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="27">
+        <v>15.96774193548387</v>
+      </c>
+      <c r="C25" s="27">
+        <v>20.225806451612904</v>
+      </c>
+      <c r="D25" s="27">
+        <v>1865.7741935483871</v>
+      </c>
+      <c r="E25" s="27">
+        <v>250.03225806451613</v>
+      </c>
+      <c r="F25" s="28">
+        <v>44.617236553662309</v>
+      </c>
+      <c r="G25" s="28">
+        <v>88.185309621704178</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="27">
+        <v>24.129032258064516</v>
+      </c>
+      <c r="K25" s="27">
+        <v>13.612903225806452</v>
+      </c>
+      <c r="L25" s="27">
+        <v>1872.3870967741937</v>
+      </c>
+      <c r="M25" s="27">
+        <v>241.87096774193549</v>
+      </c>
+      <c r="N25" s="28">
+        <v>64.450381440954075</v>
+      </c>
+      <c r="O25" s="28">
+        <v>88.562149169892677</v>
+      </c>
+      <c r="P25" s="27">
+        <v>17.870967741935484</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="V25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="W25" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="T26" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="U26" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="W26" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="V27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="W27" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="T28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="U28" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="V28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="W28" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T29" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="V29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="W29" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="U30" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="V30" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="W30" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="U31" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="V31" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="W31" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="U32" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="V32" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="W32" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="T33" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="U33" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="V33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="W33" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="T34" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="U34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="V34" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="W34" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S35" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="T35" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U35" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="V35" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="W35" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="I10:P10"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="I19:P19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new roadway feature variables from etrims data. But the data may be unusable, will have to update
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D400114C-B476-432C-A74C-BEBCF0987780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA5E50B-D54B-4244-A97C-8933F5062EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Numbers" sheetId="1" r:id="rId1"/>
-    <sheet name="Trimmed Version Break" sheetId="3" r:id="rId2"/>
+    <sheet name="Trimmed Version" sheetId="3" r:id="rId2"/>
+    <sheet name="New RoadwayVars Trimmed" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="53">
   <si>
     <t>TP</t>
   </si>
@@ -224,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +259,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -404,6 +423,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2333,8 +2384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EEF8CF-29A3-49DF-A898-012230C01B0E}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,4 +3985,305 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51C0A79-429A-4298-BF60-9C3532A4159E}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="55">
+        <v>16.580645161290324</v>
+      </c>
+      <c r="C3" s="55">
+        <v>20.419354838709676</v>
+      </c>
+      <c r="D3" s="55">
+        <v>2004.7096774193549</v>
+      </c>
+      <c r="E3" s="55">
+        <v>110.29032258064517</v>
+      </c>
+      <c r="F3" s="56">
+        <v>44.63462751304634</v>
+      </c>
+      <c r="G3" s="56">
+        <v>94.785429288856022</v>
+      </c>
+      <c r="H3" s="55">
+        <v>11.935483870967742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="60"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="63"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="46"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="55"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="60"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="63"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="46"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="46"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="57"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="60"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A15:H15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New tests with the individualized etrims intersection variables
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA5E50B-D54B-4244-A97C-8933F5062EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2898A7D5-501E-4ACA-8DB4-C1CF9F9FFB8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="68">
   <si>
     <t>TP</t>
   </si>
@@ -194,6 +194,51 @@
   </si>
   <si>
     <t>NTP</t>
+  </si>
+  <si>
+    <t>oneWayStop</t>
+  </si>
+  <si>
+    <t>oneWayStopCount</t>
+  </si>
+  <si>
+    <t>twoWayStop</t>
+  </si>
+  <si>
+    <t>twoWayStopCount</t>
+  </si>
+  <si>
+    <t>oneWayYield</t>
+  </si>
+  <si>
+    <t>oneWayYieldCount</t>
+  </si>
+  <si>
+    <t>twoWayYield</t>
+  </si>
+  <si>
+    <t>twoWayYieldCount</t>
+  </si>
+  <si>
+    <t>threeWayStop</t>
+  </si>
+  <si>
+    <t>threeWayStopCount</t>
+  </si>
+  <si>
+    <t>fourWayStop</t>
+  </si>
+  <si>
+    <t>fourWayStopCount</t>
+  </si>
+  <si>
+    <t>trafficSignal</t>
+  </si>
+  <si>
+    <t>trafficSignalCount</t>
+  </si>
+  <si>
+    <t>All Variables</t>
   </si>
 </sst>
 </file>
@@ -365,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -405,6 +450,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -423,16 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -444,17 +500,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,25 +856,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="I1" s="38" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="I1" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
       <c r="R1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1277,25 +1330,25 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="I10" s="37" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="I10" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
       <c r="R10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1742,25 +1795,25 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="I19" s="40" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="I19" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="42"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="60"/>
       <c r="R19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2385,7 +2438,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="A1:XFD1048576"/>
+      <selection activeCell="V1" sqref="V1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,25 +2464,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="I1" s="38" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="I1" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
       <c r="R1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2885,25 +2938,25 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="I10" s="37" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="I10" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
       <c r="R10" s="1" t="s">
         <v>16</v>
       </c>
@@ -3350,25 +3403,25 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="I19" s="40" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="I19" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="42"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="60"/>
       <c r="R19" s="1" t="s">
         <v>25</v>
       </c>
@@ -3989,10 +4042,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51C0A79-429A-4298-BF60-9C3532A4159E}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4006,21 +4059,34 @@
     <col min="7" max="7" width="11.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="10" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="J1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -4043,68 +4109,156 @@
       <c r="H2" s="33" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="55">
-        <v>16.580645161290324</v>
-      </c>
-      <c r="C3" s="55">
-        <v>20.419354838709676</v>
-      </c>
-      <c r="D3" s="55">
-        <v>2004.7096774193549</v>
-      </c>
-      <c r="E3" s="55">
-        <v>110.29032258064517</v>
-      </c>
-      <c r="F3" s="56">
-        <v>44.63462751304634</v>
-      </c>
-      <c r="G3" s="56">
-        <v>94.785429288856022</v>
-      </c>
-      <c r="H3" s="55">
-        <v>11.935483870967742</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="B3" s="45">
+        <v>19.806451612903224</v>
+      </c>
+      <c r="C3" s="45">
+        <v>17.451612903225808</v>
+      </c>
+      <c r="D3" s="45">
+        <v>1957.0322580645161</v>
+      </c>
+      <c r="E3" s="45">
+        <v>157.70967741935485</v>
+      </c>
+      <c r="F3" s="46">
+        <v>53.438662357869163</v>
+      </c>
+      <c r="G3" s="46">
+        <v>92.544199167349944</v>
+      </c>
+      <c r="H3" s="45">
+        <v>14.612903225806452</v>
+      </c>
+      <c r="J3" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="60"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="B4" s="50">
+        <v>20.161290322580644</v>
+      </c>
+      <c r="C4" s="50">
+        <v>17.096774193548388</v>
+      </c>
+      <c r="D4" s="50">
+        <v>1955.8064516129032</v>
+      </c>
+      <c r="E4" s="50">
+        <v>158.93548387096774</v>
+      </c>
+      <c r="F4" s="51">
+        <v>54.35144389343462</v>
+      </c>
+      <c r="G4" s="51">
+        <v>92.486239601243156</v>
+      </c>
+      <c r="H4" s="50">
+        <v>14.806451612903226</v>
+      </c>
+      <c r="J4" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="63"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="53">
+        <v>28.161290322580644</v>
+      </c>
+      <c r="C5" s="53">
+        <v>9.9032258064516121</v>
+      </c>
+      <c r="D5" s="53">
+        <v>1715.1612903225807</v>
+      </c>
+      <c r="E5" s="53">
+        <v>398.77419354838707</v>
+      </c>
+      <c r="F5" s="54">
+        <v>74.21337401264978</v>
+      </c>
+      <c r="G5" s="54">
+        <v>81.140035503194852</v>
+      </c>
+      <c r="H5" s="53">
+        <v>21.225806451612904</v>
+      </c>
+      <c r="J5" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="46"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="40"/>
+      <c r="J6" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -4113,170 +4267,830 @@
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
       <c r="H7" s="35"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="J7" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="72" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="44" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="J8" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="72" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="50" t="s">
+      <c r="H9" s="43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="J9" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="72" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="55"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="B10" s="47">
+        <v>11.096774193548388</v>
+      </c>
+      <c r="C10" s="47">
+        <v>25.483870967741936</v>
+      </c>
+      <c r="D10" s="47">
+        <v>2070.2903225806454</v>
+      </c>
+      <c r="E10" s="47">
+        <v>45.12903225806452</v>
+      </c>
+      <c r="F10" s="48">
+        <v>30.468399103486856</v>
+      </c>
+      <c r="G10" s="48">
+        <v>97.867665031678797</v>
+      </c>
+      <c r="H10" s="45">
+        <v>7.5483870967741939</v>
+      </c>
+      <c r="J10" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="60"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
+      <c r="B11" s="50">
+        <v>11.225806451612904</v>
+      </c>
+      <c r="C11" s="50">
+        <v>25.387096774193548</v>
+      </c>
+      <c r="D11" s="50">
+        <v>2069.7096774193546</v>
+      </c>
+      <c r="E11" s="50">
+        <v>45.677419354838712</v>
+      </c>
+      <c r="F11" s="51">
+        <v>30.748763742948977</v>
+      </c>
+      <c r="G11" s="51">
+        <v>97.841542768418094</v>
+      </c>
+      <c r="H11" s="50">
+        <v>7.774193548387097</v>
+      </c>
+      <c r="J11" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="72" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="63"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="46"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="46"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="B12" s="53">
+        <v>17.838709677419356</v>
+      </c>
+      <c r="C12" s="53">
+        <v>19.258064516129032</v>
+      </c>
+      <c r="D12" s="53">
+        <v>1998.1935483870968</v>
+      </c>
+      <c r="E12" s="53">
+        <v>116.70967741935483</v>
+      </c>
+      <c r="F12" s="54">
+        <v>47.906204177234557</v>
+      </c>
+      <c r="G12" s="54">
+        <v>94.482959250262354</v>
+      </c>
+      <c r="H12" s="53">
+        <v>12.838709677419354</v>
+      </c>
+      <c r="J12" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="40"/>
+      <c r="J13" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="40"/>
+      <c r="J14" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="44" t="s">
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64"/>
+      <c r="J15" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="72" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
+      <c r="B16" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="54" t="s">
+      <c r="J16" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="57"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="B17" s="47">
+        <v>16.483870967741936</v>
+      </c>
+      <c r="C17" s="47">
+        <v>20.483870967741936</v>
+      </c>
+      <c r="D17" s="47">
+        <v>2015.8387096774193</v>
+      </c>
+      <c r="E17" s="47">
+        <v>99.193548387096769</v>
+      </c>
+      <c r="F17" s="48">
+        <v>44.49087983023874</v>
+      </c>
+      <c r="G17" s="48">
+        <v>95.311611627105052</v>
+      </c>
+      <c r="H17" s="47">
+        <v>11.64516129032258</v>
+      </c>
+      <c r="J17" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="72" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="60"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="62" t="s">
+      <c r="B18" s="50">
+        <v>16.548387096774192</v>
+      </c>
+      <c r="C18" s="50">
+        <v>20.451612903225808</v>
+      </c>
+      <c r="D18" s="50">
+        <v>2013</v>
+      </c>
+      <c r="E18" s="50">
+        <v>102</v>
+      </c>
+      <c r="F18" s="51">
+        <v>44.612340749371739</v>
+      </c>
+      <c r="G18" s="51">
+        <v>95.178815149836439</v>
+      </c>
+      <c r="H18" s="50">
+        <v>11.741935483870968</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="72" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="63"/>
+      <c r="B19" s="53">
+        <v>24.483870967741936</v>
+      </c>
+      <c r="C19" s="53">
+        <v>13.096774193548388</v>
+      </c>
+      <c r="D19" s="53">
+        <v>1860.4193548387098</v>
+      </c>
+      <c r="E19" s="53">
+        <v>254</v>
+      </c>
+      <c r="F19" s="54">
+        <v>65.423376854408005</v>
+      </c>
+      <c r="G19" s="54">
+        <v>87.98955867696003</v>
+      </c>
+      <c r="H19" s="53">
+        <v>17.93548387096774</v>
+      </c>
+      <c r="J19" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" s="72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J20" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="72" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J21" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J22" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" s="66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J23" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J24" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="M24" s="66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J25" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" s="66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J26" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J27" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="L27" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J28" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" s="66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J30" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J31" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J32" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J33" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J34" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J35" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J36" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="K36" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="M36" s="66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J37" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="M37" s="66" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J38" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="M38" s="66" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J39" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="K39" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="M39" s="66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J40" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="L40" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="M40" s="66" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J41" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="K41" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="L41" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="M41" s="66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J42" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="K42" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="L42" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="M42" s="66" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J43" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="K43" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="L43" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="M43" s="66" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J44" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="K44" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="L44" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="M44" s="66" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J45" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="K45" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="L45" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="M45" s="66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J46" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="L46" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="M46" s="66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J47" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="L47" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="M47" s="66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J48" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="K48" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="L48" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="M48" s="66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J49" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="K49" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="L49" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="M49" s="66" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4285,5 +5099,6 @@
     <mergeCell ref="A15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Did more etrims intersection variable testing, no worthwhile results. Also compiled some photos of inconsistencies between cdot and etrims stop sign count datasets with google maps images.
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
+++ b/Main Dir/Logistic Regression Tests/2021 Predictions.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2898A7D5-501E-4ACA-8DB4-C1CF9F9FFB8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743DDEAE-EF87-4D3E-9AA9-864B7343B82C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{72C6B2CC-203C-463D-8B15-80DACA76F200}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Numbers" sheetId="1" r:id="rId1"/>
     <sheet name="Trimmed Version" sheetId="3" r:id="rId2"/>
     <sheet name="New RoadwayVars Trimmed" sheetId="4" r:id="rId3"/>
+    <sheet name="No ETrims or CDOT Data" sheetId="5" r:id="rId4"/>
+    <sheet name="Comparison" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="74">
   <si>
     <t>TP</t>
   </si>
@@ -240,6 +242,24 @@
   <si>
     <t>All Variables</t>
   </si>
+  <si>
+    <t>No Etrims Intersection Data</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T2 V2</t>
+  </si>
+  <si>
+    <t>T2 V3</t>
+  </si>
+  <si>
+    <t>Etrims Intersection Data (Count)</t>
+  </si>
+  <si>
+    <t>Etrims Intersection Data (Binary)</t>
+  </si>
 </sst>
 </file>
 
@@ -270,7 +290,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +342,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -470,6 +502,17 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,14 +543,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,6 +565,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF00FFFF"/>
       <color rgb="FFFF99FF"/>
     </mruColors>
   </colors>
@@ -856,25 +907,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="I1" s="56" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="I1" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
       <c r="R1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1330,25 +1381,25 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="I10" s="55" t="s">
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="I10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
       <c r="R10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1795,25 +1846,25 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="I19" s="58" t="s">
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="I19" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="60"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="71"/>
       <c r="R19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2464,25 +2515,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="I1" s="56" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="I1" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
       <c r="R1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2938,25 +2989,25 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="I10" s="55" t="s">
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="I10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
       <c r="R10" s="1" t="s">
         <v>16</v>
       </c>
@@ -3403,25 +3454,25 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="I19" s="58" t="s">
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="I19" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="60"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="71"/>
       <c r="R19" s="1" t="s">
         <v>25</v>
       </c>
@@ -4042,10 +4093,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51C0A79-429A-4298-BF60-9C3532A4159E}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4059,20 +4110,20 @@
     <col min="7" max="7" width="11.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
       <c r="J1" s="7" t="s">
         <v>67</v>
       </c>
@@ -4085,8 +4136,17 @@
       <c r="M1" s="52" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -4112,17 +4172,26 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="69" t="s">
+      <c r="L2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="71" t="s">
+      <c r="M2" s="61" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>6</v>
       </c>
@@ -4147,20 +4216,29 @@
       <c r="H3" s="45">
         <v>14.612903225806452</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="68" t="s">
+      <c r="K3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="70" t="s">
+      <c r="L3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="72" t="s">
+      <c r="M3" s="62" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="83" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="87" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>42</v>
       </c>
@@ -4185,20 +4263,29 @@
       <c r="H4" s="50">
         <v>14.806451612903226</v>
       </c>
-      <c r="J4" s="65" t="s">
+      <c r="J4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="68" t="s">
+      <c r="K4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="70" t="s">
+      <c r="L4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="72" t="s">
+      <c r="M4" s="62" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="83" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="87" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>43</v>
       </c>
@@ -4223,20 +4310,1642 @@
       <c r="H5" s="53">
         <v>21.225806451612904</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="68" t="s">
+      <c r="K5" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="70" t="s">
+      <c r="L5" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="72" t="s">
+      <c r="M5" s="62" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="83" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="85" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="87" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="27">
+        <v>21.322580645161292</v>
+      </c>
+      <c r="C6" s="27">
+        <v>16.225806451612904</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1933</v>
+      </c>
+      <c r="E6" s="27">
+        <v>181.45161290322579</v>
+      </c>
+      <c r="F6" s="28">
+        <v>56.999645890984183</v>
+      </c>
+      <c r="G6" s="28">
+        <v>91.42126006465493</v>
+      </c>
+      <c r="H6" s="27">
+        <v>15.193548387096774</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="78">
+        <v>21.096774193548388</v>
+      </c>
+      <c r="C7" s="78">
+        <v>16.483870967741936</v>
+      </c>
+      <c r="D7" s="78">
+        <v>1929.6451612903227</v>
+      </c>
+      <c r="E7" s="78">
+        <v>184.7741935483871</v>
+      </c>
+      <c r="F7" s="79">
+        <v>56.496353729419482</v>
+      </c>
+      <c r="G7" s="79">
+        <v>91.264149956436526</v>
+      </c>
+      <c r="H7" s="78">
+        <v>15.064516129032258</v>
+      </c>
+      <c r="J7" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="87" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="81">
+        <v>30.580645161290324</v>
+      </c>
+      <c r="C8" s="81">
+        <v>7.903225806451613</v>
+      </c>
+      <c r="D8" s="81">
+        <v>1669.7741935483871</v>
+      </c>
+      <c r="E8" s="81">
+        <v>443.74193548387098</v>
+      </c>
+      <c r="F8" s="82">
+        <v>79.660477408666225</v>
+      </c>
+      <c r="G8" s="82">
+        <v>79.007895656432154</v>
+      </c>
+      <c r="H8" s="81">
+        <v>23</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="40"/>
+      <c r="J9" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="35"/>
+      <c r="J10" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="87" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="75"/>
+      <c r="J11" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
+      <c r="B12" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="87" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="47">
+        <v>11.096774193548388</v>
+      </c>
+      <c r="C13" s="47">
+        <v>25.483870967741936</v>
+      </c>
+      <c r="D13" s="47">
+        <v>2070.2903225806454</v>
+      </c>
+      <c r="E13" s="47">
+        <v>45.12903225806452</v>
+      </c>
+      <c r="F13" s="48">
+        <v>30.468399103486856</v>
+      </c>
+      <c r="G13" s="48">
+        <v>97.867665031678797</v>
+      </c>
+      <c r="H13" s="45">
+        <v>7.5483870967741939</v>
+      </c>
+      <c r="J13" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="83" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="87" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="50">
+        <v>11.225806451612904</v>
+      </c>
+      <c r="C14" s="50">
+        <v>25.387096774193548</v>
+      </c>
+      <c r="D14" s="50">
+        <v>2069.7096774193546</v>
+      </c>
+      <c r="E14" s="50">
+        <v>45.677419354838712</v>
+      </c>
+      <c r="F14" s="51">
+        <v>30.748763742948977</v>
+      </c>
+      <c r="G14" s="51">
+        <v>97.841542768418094</v>
+      </c>
+      <c r="H14" s="50">
+        <v>7.774193548387097</v>
+      </c>
+      <c r="J14" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" s="87" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="53">
+        <v>17.838709677419356</v>
+      </c>
+      <c r="C15" s="53">
+        <v>19.258064516129032</v>
+      </c>
+      <c r="D15" s="53">
+        <v>1998.1935483870968</v>
+      </c>
+      <c r="E15" s="53">
+        <v>116.70967741935483</v>
+      </c>
+      <c r="F15" s="54">
+        <v>47.906204177234557</v>
+      </c>
+      <c r="G15" s="54">
+        <v>94.482959250262354</v>
+      </c>
+      <c r="H15" s="53">
+        <v>12.838709677419354</v>
+      </c>
+      <c r="J15" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" s="83" t="s">
+        <v>31</v>
+      </c>
+      <c r="O15" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="87" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="27">
+        <v>9.5161290322580641</v>
+      </c>
+      <c r="C16" s="27">
+        <v>27.096774193548388</v>
+      </c>
+      <c r="D16" s="27">
+        <v>2074.6451612903224</v>
+      </c>
+      <c r="E16" s="27">
+        <v>40.741935483870968</v>
+      </c>
+      <c r="F16" s="28">
+        <v>26.356512689644745</v>
+      </c>
+      <c r="G16" s="28">
+        <v>98.075062440896033</v>
+      </c>
+      <c r="H16" s="27">
+        <v>6.903225806451613</v>
+      </c>
+      <c r="J16" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="87" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="78">
+        <v>9.6451612903225801</v>
+      </c>
+      <c r="C17" s="78">
+        <v>27</v>
+      </c>
+      <c r="D17" s="78">
+        <v>2073.7096774193546</v>
+      </c>
+      <c r="E17" s="78">
+        <v>41.645161290322584</v>
+      </c>
+      <c r="F17" s="79">
+        <v>26.560037571148857</v>
+      </c>
+      <c r="G17" s="79">
+        <v>98.032205900632178</v>
+      </c>
+      <c r="H17" s="78">
+        <v>6.838709677419355</v>
+      </c>
+      <c r="J17" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17" s="83" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17" s="87" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="81">
+        <v>18.06451612903226</v>
+      </c>
+      <c r="C18" s="81">
+        <v>19.161290322580644</v>
+      </c>
+      <c r="D18" s="81">
+        <v>1984.6774193548388</v>
+      </c>
+      <c r="E18" s="81">
+        <v>130.09677419354838</v>
+      </c>
+      <c r="F18" s="82">
+        <v>48.799390451271599</v>
+      </c>
+      <c r="G18" s="82">
+        <v>93.85025580237091</v>
+      </c>
+      <c r="H18" s="81">
+        <v>12.741935483870968</v>
+      </c>
+      <c r="J18" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" s="87" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="40"/>
+      <c r="J19" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="N19" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="P19" s="87" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="P20" s="87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="75"/>
+      <c r="J21" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21" s="56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="P22" s="56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="47">
+        <v>16.483870967741936</v>
+      </c>
+      <c r="C23" s="47">
+        <v>20.483870967741936</v>
+      </c>
+      <c r="D23" s="47">
+        <v>2015.8387096774193</v>
+      </c>
+      <c r="E23" s="47">
+        <v>99.193548387096769</v>
+      </c>
+      <c r="F23" s="48">
+        <v>44.49087983023874</v>
+      </c>
+      <c r="G23" s="48">
+        <v>95.311611627105052</v>
+      </c>
+      <c r="H23" s="47">
+        <v>11.64516129032258</v>
+      </c>
+      <c r="J23" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="N23" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="O23" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="P23" s="56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="50">
+        <v>16.548387096774192</v>
+      </c>
+      <c r="C24" s="50">
+        <v>20.451612903225808</v>
+      </c>
+      <c r="D24" s="50">
+        <v>2013</v>
+      </c>
+      <c r="E24" s="50">
+        <v>102</v>
+      </c>
+      <c r="F24" s="51">
+        <v>44.612340749371739</v>
+      </c>
+      <c r="G24" s="51">
+        <v>95.178815149836439</v>
+      </c>
+      <c r="H24" s="50">
+        <v>11.741935483870968</v>
+      </c>
+      <c r="J24" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="M24" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="O24" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="P24" s="56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="53">
+        <v>24.483870967741936</v>
+      </c>
+      <c r="C25" s="53">
+        <v>13.096774193548388</v>
+      </c>
+      <c r="D25" s="53">
+        <v>1860.4193548387098</v>
+      </c>
+      <c r="E25" s="53">
+        <v>254</v>
+      </c>
+      <c r="F25" s="54">
+        <v>65.423376854408005</v>
+      </c>
+      <c r="G25" s="54">
+        <v>87.98955867696003</v>
+      </c>
+      <c r="H25" s="53">
+        <v>17.93548387096774</v>
+      </c>
+      <c r="J25" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="O25" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="P25" s="56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="27">
+        <v>16.193548387096776</v>
+      </c>
+      <c r="C26" s="27">
+        <v>20.93548387096774</v>
+      </c>
+      <c r="D26" s="27">
+        <v>2002.9032258064517</v>
+      </c>
+      <c r="E26" s="27">
+        <v>111.96774193548387</v>
+      </c>
+      <c r="F26" s="28">
+        <v>43.60926001088756</v>
+      </c>
+      <c r="G26" s="28">
+        <v>94.707684024259223</v>
+      </c>
+      <c r="H26" s="27">
+        <v>11.064516129032258</v>
+      </c>
+      <c r="J26" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="83" t="s">
+        <v>59</v>
+      </c>
+      <c r="O26" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="P26" s="56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="78">
+        <v>16.032258064516128</v>
+      </c>
+      <c r="C27" s="78">
+        <v>21.06451612903226</v>
+      </c>
+      <c r="D27" s="78">
+        <v>1999.6129032258063</v>
+      </c>
+      <c r="E27" s="78">
+        <v>115.29032258064517</v>
+      </c>
+      <c r="F27" s="79">
+        <v>43.314489970866902</v>
+      </c>
+      <c r="G27" s="79">
+        <v>94.550851517970969</v>
+      </c>
+      <c r="H27" s="78">
+        <v>11.129032258064516</v>
+      </c>
+      <c r="J27" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="L27" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="N27" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="O27" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="P27" s="56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="81">
+        <v>26.70967741935484</v>
+      </c>
+      <c r="C28" s="81">
+        <v>11.32258064516129</v>
+      </c>
+      <c r="D28" s="81">
+        <v>1822.258064516129</v>
+      </c>
+      <c r="E28" s="81">
+        <v>291.70967741935482</v>
+      </c>
+      <c r="F28" s="82">
+        <v>70.491031901416775</v>
+      </c>
+      <c r="G28" s="82">
+        <v>86.203461656902974</v>
+      </c>
+      <c r="H28" s="81">
+        <v>19.774193548387096</v>
+      </c>
+      <c r="J28" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="O28" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="P28" s="56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J29" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="N29" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="O29" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="P29" s="56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J30" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="P30" s="56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J31" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="O31" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="P31" s="56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J32" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="O32" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P32" s="56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J33" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="N33" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="O33" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="P33" s="56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J34" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="N34" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="P34" s="56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J35" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="N35" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="O35" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="P35" s="56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J36" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="K36" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="M36" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="N36" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="P36" s="56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J37" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="M37" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="N37" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="O37" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="P37" s="56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J38" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="M38" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="N38" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="O38" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="P38" s="56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J39" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K39" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="M39" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="N39" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="O39" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="P39" s="56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J40" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="L40" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="M40" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="N40" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="P40" s="56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J41" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="K41" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="L41" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="M41" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="N41" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="O41" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="P41" s="56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J42" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="K42" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="L42" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="M42" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="N42" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="P42" s="56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J43" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K43" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="L43" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="M43" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="N43" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="O43" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="P43" s="56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J44" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="K44" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="L44" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="M44" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="N44" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="O44" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="P44" s="56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J45" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="K45" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="L45" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="M45" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="N45" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="O45" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="P45" s="56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J46" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="L46" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="M46" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="N46" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="O46" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="P46" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J47" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="L47" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="M47" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="N47" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="O47" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="P47" s="56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J48" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="K48" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="L48" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="M48" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="O48" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="P48" s="56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J49" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="K49" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="L49" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="M49" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="N49" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="O49" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="P49" s="56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A21:H21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23394318-67EE-4921-BA37-9F947F069624}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="64">
+        <v>19.93548387096774</v>
+      </c>
+      <c r="C3" s="64">
+        <v>17.29032258064516</v>
+      </c>
+      <c r="D3" s="64">
+        <v>1967.8064516129032</v>
+      </c>
+      <c r="E3" s="64">
+        <v>146.96774193548387</v>
+      </c>
+      <c r="F3" s="65">
+        <v>53.415036045937562</v>
+      </c>
+      <c r="G3" s="65">
+        <v>93.052301827539608</v>
+      </c>
+      <c r="H3" s="64">
+        <v>14.419354838709678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="38">
+        <v>19.903225806451612</v>
+      </c>
+      <c r="C4" s="38">
+        <v>17.322580645161292</v>
+      </c>
+      <c r="D4" s="38">
+        <v>1970.2903225806451</v>
+      </c>
+      <c r="E4" s="38">
+        <v>144.48387096774192</v>
+      </c>
+      <c r="F4" s="39">
+        <v>53.322870147320046</v>
+      </c>
+      <c r="G4" s="39">
+        <v>93.16969443333511</v>
+      </c>
+      <c r="H4" s="38">
+        <v>14.451612903225806</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="38">
+        <v>26.967741935483872</v>
+      </c>
+      <c r="C5" s="38">
+        <v>11.129032258064516</v>
+      </c>
+      <c r="D5" s="38">
+        <v>1764.8387096774193</v>
+      </c>
+      <c r="E5" s="38">
+        <v>349.06451612903226</v>
+      </c>
+      <c r="F5" s="39">
+        <v>71.191142849846955</v>
+      </c>
+      <c r="G5" s="39">
+        <v>83.491755068955101</v>
+      </c>
+      <c r="H5" s="38">
+        <v>20.419354838709676</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -4245,20 +5954,8 @@
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
       <c r="H6" s="40"/>
-      <c r="J6" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="72" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -4267,44 +5964,20 @@
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
       <c r="H7" s="35"/>
-      <c r="J7" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="68" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" s="72" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="J8" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="72" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="38" t="s">
         <v>0</v>
@@ -4327,134 +6000,86 @@
       <c r="H9" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="72" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="47">
-        <v>11.096774193548388</v>
-      </c>
-      <c r="C10" s="47">
-        <v>25.483870967741936</v>
-      </c>
-      <c r="D10" s="47">
-        <v>2070.2903225806454</v>
-      </c>
-      <c r="E10" s="47">
-        <v>45.12903225806452</v>
-      </c>
-      <c r="F10" s="48">
-        <v>30.468399103486856</v>
-      </c>
-      <c r="G10" s="48">
-        <v>97.867665031678797</v>
-      </c>
-      <c r="H10" s="45">
-        <v>7.5483870967741939</v>
-      </c>
-      <c r="J10" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="72" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="B10" s="38">
+        <v>11.67741935483871</v>
+      </c>
+      <c r="C10" s="38">
+        <v>24.903225806451612</v>
+      </c>
+      <c r="D10" s="38">
+        <v>2067.0322580645161</v>
+      </c>
+      <c r="E10" s="38">
+        <v>48.387096774193552</v>
+      </c>
+      <c r="F10" s="39">
+        <v>31.894561615054943</v>
+      </c>
+      <c r="G10" s="39">
+        <v>97.713455884708779</v>
+      </c>
+      <c r="H10" s="64">
+        <v>8.2258064516129039</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="50">
-        <v>11.225806451612904</v>
-      </c>
-      <c r="C11" s="50">
-        <v>25.387096774193548</v>
-      </c>
-      <c r="D11" s="50">
-        <v>2069.7096774193546</v>
-      </c>
-      <c r="E11" s="50">
-        <v>45.677419354838712</v>
-      </c>
-      <c r="F11" s="51">
-        <v>30.748763742948977</v>
-      </c>
-      <c r="G11" s="51">
-        <v>97.841542768418094</v>
-      </c>
-      <c r="H11" s="50">
-        <v>7.774193548387097</v>
-      </c>
-      <c r="J11" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="68" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" s="72" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+      <c r="B11" s="38">
+        <v>11.548387096774194</v>
+      </c>
+      <c r="C11" s="38">
+        <v>25.032258064516128</v>
+      </c>
+      <c r="D11" s="38">
+        <v>2068.0967741935483</v>
+      </c>
+      <c r="E11" s="38">
+        <v>47.322580645161288</v>
+      </c>
+      <c r="F11" s="39">
+        <v>31.386501662885241</v>
+      </c>
+      <c r="G11" s="39">
+        <v>97.76378691728371</v>
+      </c>
+      <c r="H11" s="38">
+        <v>8.129032258064516</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="53">
-        <v>17.838709677419356</v>
-      </c>
-      <c r="C12" s="53">
-        <v>19.258064516129032</v>
-      </c>
-      <c r="D12" s="53">
-        <v>1998.1935483870968</v>
-      </c>
-      <c r="E12" s="53">
-        <v>116.70967741935483</v>
-      </c>
-      <c r="F12" s="54">
-        <v>47.906204177234557</v>
-      </c>
-      <c r="G12" s="54">
-        <v>94.482959250262354</v>
-      </c>
-      <c r="H12" s="53">
-        <v>12.838709677419354</v>
-      </c>
-      <c r="J12" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="72" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="38">
+        <v>17.516129032258064</v>
+      </c>
+      <c r="C12" s="38">
+        <v>19.451612903225808</v>
+      </c>
+      <c r="D12" s="38">
+        <v>2012.6451612903227</v>
+      </c>
+      <c r="E12" s="38">
+        <v>102.38709677419355</v>
+      </c>
+      <c r="F12" s="39">
+        <v>47.15706021024382</v>
+      </c>
+      <c r="G12" s="39">
+        <v>95.160262901923915</v>
+      </c>
+      <c r="H12" s="38">
+        <v>12.64516129032258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -4463,20 +6088,8 @@
       <c r="F13" s="41"/>
       <c r="G13" s="41"/>
       <c r="H13" s="40"/>
-      <c r="J13" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="72" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
@@ -4485,44 +6098,20 @@
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
       <c r="H14" s="40"/>
-      <c r="J14" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="72" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="62" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="64"/>
-      <c r="J15" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="L15" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" s="72" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="75"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
       <c r="B16" s="38" t="s">
         <v>0</v>
@@ -4545,551 +6134,83 @@
       <c r="H16" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="72" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="47">
-        <v>16.483870967741936</v>
-      </c>
-      <c r="C17" s="47">
-        <v>20.483870967741936</v>
-      </c>
-      <c r="D17" s="47">
-        <v>2015.8387096774193</v>
-      </c>
-      <c r="E17" s="47">
-        <v>99.193548387096769</v>
-      </c>
-      <c r="F17" s="48">
-        <v>44.49087983023874</v>
-      </c>
-      <c r="G17" s="48">
-        <v>95.311611627105052</v>
-      </c>
-      <c r="H17" s="47">
-        <v>11.64516129032258</v>
-      </c>
-      <c r="J17" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="L17" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="72" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="B17" s="38">
+        <v>16.741935483870968</v>
+      </c>
+      <c r="C17" s="38">
+        <v>20.225806451612904</v>
+      </c>
+      <c r="D17" s="38">
+        <v>2018.5806451612902</v>
+      </c>
+      <c r="E17" s="38">
+        <v>96.451612903225808</v>
+      </c>
+      <c r="F17" s="39">
+        <v>45.220546115446808</v>
+      </c>
+      <c r="G17" s="39">
+        <v>95.441024617958405</v>
+      </c>
+      <c r="H17" s="38">
+        <v>12.258064516129032</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="50">
-        <v>16.548387096774192</v>
-      </c>
-      <c r="C18" s="50">
-        <v>20.451612903225808</v>
-      </c>
-      <c r="D18" s="50">
-        <v>2013</v>
-      </c>
-      <c r="E18" s="50">
-        <v>102</v>
-      </c>
-      <c r="F18" s="51">
-        <v>44.612340749371739</v>
-      </c>
-      <c r="G18" s="51">
-        <v>95.178815149836439</v>
-      </c>
-      <c r="H18" s="50">
-        <v>11.741935483870968</v>
-      </c>
-      <c r="J18" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="M18" s="72" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+      <c r="B18" s="38">
+        <v>16.70967741935484</v>
+      </c>
+      <c r="C18" s="38">
+        <v>20.258064516129032</v>
+      </c>
+      <c r="D18" s="38">
+        <v>2020.3225806451612</v>
+      </c>
+      <c r="E18" s="38">
+        <v>94.709677419354833</v>
+      </c>
+      <c r="F18" s="39">
+        <v>45.153341814371537</v>
+      </c>
+      <c r="G18" s="39">
+        <v>95.523327653158304</v>
+      </c>
+      <c r="H18" s="38">
+        <v>12.258064516129032</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="53">
-        <v>24.483870967741936</v>
-      </c>
-      <c r="C19" s="53">
-        <v>13.096774193548388</v>
-      </c>
-      <c r="D19" s="53">
-        <v>1860.4193548387098</v>
-      </c>
-      <c r="E19" s="53">
-        <v>254</v>
-      </c>
-      <c r="F19" s="54">
-        <v>65.423376854408005</v>
-      </c>
-      <c r="G19" s="54">
-        <v>87.98955867696003</v>
-      </c>
-      <c r="H19" s="53">
-        <v>17.93548387096774</v>
-      </c>
-      <c r="J19" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" s="72" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="L20" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="M20" s="72" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J21" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="K21" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="L21" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="M21" s="72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J22" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="K22" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="L22" s="70" t="s">
-        <v>58</v>
-      </c>
-      <c r="M22" s="66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J23" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="K23" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="L23" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="M23" s="66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J24" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="K24" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="L24" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="M24" s="66" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J25" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="K25" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="L25" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="M25" s="66" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J26" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="M26" s="66" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J27" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="K27" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="L27" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="66" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J28" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="K28" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="L28" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="M28" s="66" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J29" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="K29" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="L29" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="M29" s="66" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J30" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="K30" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="L30" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="66" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J31" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="K31" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="L31" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="66" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J32" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="K32" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" s="66" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J33" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="K33" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="L33" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="M33" s="66" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J34" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="L34" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="M34" s="66" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="K35" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="L35" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="M35" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J36" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="K36" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="L36" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="M36" s="66" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J37" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="K37" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="L37" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="M37" s="66" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J38" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="K38" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="L38" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="M38" s="66" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J39" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="K39" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="L39" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="M39" s="66" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="K40" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="L40" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="M40" s="66" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J41" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="K41" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="L41" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="M41" s="66" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J42" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="K42" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="L42" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="M42" s="66" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J43" s="65" t="s">
-        <v>60</v>
-      </c>
-      <c r="K43" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="L43" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="M43" s="66" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J44" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="K44" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="L44" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="M44" s="66" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J45" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="K45" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="L45" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="M45" s="66" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J46" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="K46" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="L46" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="M46" s="66" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J47" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="K47" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="L47" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="M47" s="66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J48" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="K48" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="L48" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="M48" s="66" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J49" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="K49" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="L49" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="M49" s="66" t="s">
-        <v>65</v>
+      <c r="B19" s="38">
+        <v>23.129032258064516</v>
+      </c>
+      <c r="C19" s="38">
+        <v>14.516129032258064</v>
+      </c>
+      <c r="D19" s="38">
+        <v>1905.5806451612902</v>
+      </c>
+      <c r="E19" s="38">
+        <v>208.7741935483871</v>
+      </c>
+      <c r="F19" s="39">
+        <v>61.906966961525526</v>
+      </c>
+      <c r="G19" s="39">
+        <v>90.127957897689825</v>
+      </c>
+      <c r="H19" s="38">
+        <v>17.096774193548388</v>
       </c>
     </row>
   </sheetData>
@@ -5099,6 +6220,1162 @@
     <mergeCell ref="A15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2ECD78-8E2E-4BE1-9ED5-A347FB11F918}">
+  <dimension ref="A1:Z20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE31" sqref="AE31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="J1" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="S1" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="J2" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="S2" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="1"/>
+      <c r="T3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="64">
+        <v>19.806451612903224</v>
+      </c>
+      <c r="C4" s="64">
+        <v>17.451612903225808</v>
+      </c>
+      <c r="D4" s="64">
+        <v>1957.0322580645161</v>
+      </c>
+      <c r="E4" s="64">
+        <v>157.70967741935485</v>
+      </c>
+      <c r="F4" s="65">
+        <v>53.438662357869163</v>
+      </c>
+      <c r="G4" s="65">
+        <v>92.544199167349944</v>
+      </c>
+      <c r="H4" s="64">
+        <v>14.612903225806452</v>
+      </c>
+      <c r="J4" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="64">
+        <v>19.93548387096774</v>
+      </c>
+      <c r="L4" s="64">
+        <v>17.29032258064516</v>
+      </c>
+      <c r="M4" s="64">
+        <v>1967.8064516129032</v>
+      </c>
+      <c r="N4" s="64">
+        <v>146.96774193548387</v>
+      </c>
+      <c r="O4" s="65">
+        <v>53.415036045937562</v>
+      </c>
+      <c r="P4" s="65">
+        <v>93.052301827539608</v>
+      </c>
+      <c r="Q4" s="64">
+        <v>14.419354838709678</v>
+      </c>
+      <c r="S4" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="38">
+        <v>21.322580645161292</v>
+      </c>
+      <c r="U4" s="38">
+        <v>16.225806451612904</v>
+      </c>
+      <c r="V4" s="38">
+        <v>1933</v>
+      </c>
+      <c r="W4" s="38">
+        <v>181.45161290322579</v>
+      </c>
+      <c r="X4" s="39">
+        <v>56.999645890984183</v>
+      </c>
+      <c r="Y4" s="39">
+        <v>91.42126006465493</v>
+      </c>
+      <c r="Z4" s="38">
+        <v>15.193548387096774</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="38">
+        <v>20.161290322580644</v>
+      </c>
+      <c r="C5" s="38">
+        <v>17.096774193548388</v>
+      </c>
+      <c r="D5" s="38">
+        <v>1955.8064516129032</v>
+      </c>
+      <c r="E5" s="38">
+        <v>158.93548387096774</v>
+      </c>
+      <c r="F5" s="39">
+        <v>54.35144389343462</v>
+      </c>
+      <c r="G5" s="39">
+        <v>92.486239601243156</v>
+      </c>
+      <c r="H5" s="38">
+        <v>14.806451612903226</v>
+      </c>
+      <c r="J5" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="38">
+        <v>19.903225806451612</v>
+      </c>
+      <c r="L5" s="38">
+        <v>17.322580645161292</v>
+      </c>
+      <c r="M5" s="38">
+        <v>1970.2903225806451</v>
+      </c>
+      <c r="N5" s="38">
+        <v>144.48387096774192</v>
+      </c>
+      <c r="O5" s="39">
+        <v>53.322870147320046</v>
+      </c>
+      <c r="P5" s="39">
+        <v>93.16969443333511</v>
+      </c>
+      <c r="Q5" s="38">
+        <v>14.451612903225806</v>
+      </c>
+      <c r="S5" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" s="38">
+        <v>21.096774193548388</v>
+      </c>
+      <c r="U5" s="38">
+        <v>16.483870967741936</v>
+      </c>
+      <c r="V5" s="38">
+        <v>1929.6451612903227</v>
+      </c>
+      <c r="W5" s="38">
+        <v>184.7741935483871</v>
+      </c>
+      <c r="X5" s="39">
+        <v>56.496353729419482</v>
+      </c>
+      <c r="Y5" s="39">
+        <v>91.264149956436526</v>
+      </c>
+      <c r="Z5" s="38">
+        <v>15.064516129032258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="38">
+        <v>28.161290322580644</v>
+      </c>
+      <c r="C6" s="38">
+        <v>9.9032258064516121</v>
+      </c>
+      <c r="D6" s="38">
+        <v>1715.1612903225807</v>
+      </c>
+      <c r="E6" s="38">
+        <v>398.77419354838707</v>
+      </c>
+      <c r="F6" s="39">
+        <v>74.21337401264978</v>
+      </c>
+      <c r="G6" s="39">
+        <v>81.140035503194852</v>
+      </c>
+      <c r="H6" s="38">
+        <v>21.225806451612904</v>
+      </c>
+      <c r="J6" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="38">
+        <v>26.967741935483872</v>
+      </c>
+      <c r="L6" s="38">
+        <v>11.129032258064516</v>
+      </c>
+      <c r="M6" s="38">
+        <v>1764.8387096774193</v>
+      </c>
+      <c r="N6" s="38">
+        <v>349.06451612903226</v>
+      </c>
+      <c r="O6" s="39">
+        <v>71.191142849846955</v>
+      </c>
+      <c r="P6" s="39">
+        <v>83.491755068955101</v>
+      </c>
+      <c r="Q6" s="38">
+        <v>20.419354838709676</v>
+      </c>
+      <c r="S6" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="T6" s="38">
+        <v>30.580645161290324</v>
+      </c>
+      <c r="U6" s="38">
+        <v>7.903225806451613</v>
+      </c>
+      <c r="V6" s="38">
+        <v>1669.7741935483871</v>
+      </c>
+      <c r="W6" s="38">
+        <v>443.74193548387098</v>
+      </c>
+      <c r="X6" s="39">
+        <v>79.660477408666225</v>
+      </c>
+      <c r="Y6" s="39">
+        <v>79.007895656432154</v>
+      </c>
+      <c r="Z6" s="38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="40"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="40"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="40"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="35"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="35"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="36"/>
+      <c r="Z8" s="35"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="J9" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="S9" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="74"/>
+      <c r="X9" s="74"/>
+      <c r="Y9" s="74"/>
+      <c r="Z9" s="75"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="42"/>
+      <c r="K10" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="42"/>
+      <c r="T10" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="U10" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="V10" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="W10" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="X10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="38">
+        <v>11.096774193548388</v>
+      </c>
+      <c r="C11" s="38">
+        <v>25.483870967741936</v>
+      </c>
+      <c r="D11" s="38">
+        <v>2070.2903225806454</v>
+      </c>
+      <c r="E11" s="38">
+        <v>45.12903225806452</v>
+      </c>
+      <c r="F11" s="39">
+        <v>30.468399103486856</v>
+      </c>
+      <c r="G11" s="39">
+        <v>97.867665031678797</v>
+      </c>
+      <c r="H11" s="64">
+        <v>7.5483870967741939</v>
+      </c>
+      <c r="J11" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="38">
+        <v>11.67741935483871</v>
+      </c>
+      <c r="L11" s="38">
+        <v>24.903225806451612</v>
+      </c>
+      <c r="M11" s="38">
+        <v>2067.0322580645161</v>
+      </c>
+      <c r="N11" s="38">
+        <v>48.387096774193552</v>
+      </c>
+      <c r="O11" s="39">
+        <v>31.894561615054943</v>
+      </c>
+      <c r="P11" s="39">
+        <v>97.713455884708779</v>
+      </c>
+      <c r="Q11" s="64">
+        <v>8.2258064516129039</v>
+      </c>
+      <c r="S11" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" s="38">
+        <v>9.5161290322580641</v>
+      </c>
+      <c r="U11" s="38">
+        <v>27.096774193548388</v>
+      </c>
+      <c r="V11" s="38">
+        <v>2074.6451612903224</v>
+      </c>
+      <c r="W11" s="38">
+        <v>40.741935483870968</v>
+      </c>
+      <c r="X11" s="39">
+        <v>26.356512689644745</v>
+      </c>
+      <c r="Y11" s="39">
+        <v>98.075062440896033</v>
+      </c>
+      <c r="Z11" s="38">
+        <v>6.903225806451613</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="38">
+        <v>11.225806451612904</v>
+      </c>
+      <c r="C12" s="38">
+        <v>25.387096774193548</v>
+      </c>
+      <c r="D12" s="38">
+        <v>2069.7096774193546</v>
+      </c>
+      <c r="E12" s="38">
+        <v>45.677419354838712</v>
+      </c>
+      <c r="F12" s="39">
+        <v>30.748763742948977</v>
+      </c>
+      <c r="G12" s="39">
+        <v>97.841542768418094</v>
+      </c>
+      <c r="H12" s="38">
+        <v>7.774193548387097</v>
+      </c>
+      <c r="J12" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="38">
+        <v>11.548387096774194</v>
+      </c>
+      <c r="L12" s="38">
+        <v>25.032258064516128</v>
+      </c>
+      <c r="M12" s="38">
+        <v>2068.0967741935483</v>
+      </c>
+      <c r="N12" s="38">
+        <v>47.322580645161288</v>
+      </c>
+      <c r="O12" s="39">
+        <v>31.386501662885241</v>
+      </c>
+      <c r="P12" s="39">
+        <v>97.76378691728371</v>
+      </c>
+      <c r="Q12" s="38">
+        <v>8.129032258064516</v>
+      </c>
+      <c r="S12" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="T12" s="38">
+        <v>9.6451612903225801</v>
+      </c>
+      <c r="U12" s="38">
+        <v>27</v>
+      </c>
+      <c r="V12" s="38">
+        <v>2073.7096774193546</v>
+      </c>
+      <c r="W12" s="38">
+        <v>41.645161290322584</v>
+      </c>
+      <c r="X12" s="39">
+        <v>26.560037571148857</v>
+      </c>
+      <c r="Y12" s="39">
+        <v>98.032205900632178</v>
+      </c>
+      <c r="Z12" s="38">
+        <v>6.838709677419355</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="38">
+        <v>17.838709677419356</v>
+      </c>
+      <c r="C13" s="38">
+        <v>19.258064516129032</v>
+      </c>
+      <c r="D13" s="38">
+        <v>1998.1935483870968</v>
+      </c>
+      <c r="E13" s="38">
+        <v>116.70967741935483</v>
+      </c>
+      <c r="F13" s="39">
+        <v>47.906204177234557</v>
+      </c>
+      <c r="G13" s="39">
+        <v>94.482959250262354</v>
+      </c>
+      <c r="H13" s="38">
+        <v>12.838709677419354</v>
+      </c>
+      <c r="J13" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="38">
+        <v>17.516129032258064</v>
+      </c>
+      <c r="L13" s="38">
+        <v>19.451612903225808</v>
+      </c>
+      <c r="M13" s="38">
+        <v>2012.6451612903227</v>
+      </c>
+      <c r="N13" s="38">
+        <v>102.38709677419355</v>
+      </c>
+      <c r="O13" s="39">
+        <v>47.15706021024382</v>
+      </c>
+      <c r="P13" s="39">
+        <v>95.160262901923915</v>
+      </c>
+      <c r="Q13" s="38">
+        <v>12.64516129032258</v>
+      </c>
+      <c r="S13" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="T13" s="38">
+        <v>18.06451612903226</v>
+      </c>
+      <c r="U13" s="38">
+        <v>19.161290322580644</v>
+      </c>
+      <c r="V13" s="38">
+        <v>1984.6774193548388</v>
+      </c>
+      <c r="W13" s="38">
+        <v>130.09677419354838</v>
+      </c>
+      <c r="X13" s="39">
+        <v>48.799390451271599</v>
+      </c>
+      <c r="Y13" s="39">
+        <v>93.85025580237091</v>
+      </c>
+      <c r="Z13" s="38">
+        <v>12.741935483870968</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="40"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="40"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="40"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="40"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="40"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="40"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="75"/>
+      <c r="J16" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="75"/>
+      <c r="S16" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="T16" s="74"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="74"/>
+      <c r="X16" s="74"/>
+      <c r="Y16" s="74"/>
+      <c r="Z16" s="75"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="42"/>
+      <c r="B17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="42"/>
+      <c r="K17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="S17" s="42"/>
+      <c r="T17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="W17" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="X17" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z17" s="43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="38">
+        <v>16.483870967741936</v>
+      </c>
+      <c r="C18" s="38">
+        <v>20.483870967741936</v>
+      </c>
+      <c r="D18" s="38">
+        <v>2015.8387096774193</v>
+      </c>
+      <c r="E18" s="38">
+        <v>99.193548387096769</v>
+      </c>
+      <c r="F18" s="39">
+        <v>44.49087983023874</v>
+      </c>
+      <c r="G18" s="39">
+        <v>95.311611627105052</v>
+      </c>
+      <c r="H18" s="38">
+        <v>11.64516129032258</v>
+      </c>
+      <c r="J18" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="38">
+        <v>16.741935483870968</v>
+      </c>
+      <c r="L18" s="38">
+        <v>20.225806451612904</v>
+      </c>
+      <c r="M18" s="38">
+        <v>2018.5806451612902</v>
+      </c>
+      <c r="N18" s="38">
+        <v>96.451612903225808</v>
+      </c>
+      <c r="O18" s="39">
+        <v>45.220546115446808</v>
+      </c>
+      <c r="P18" s="39">
+        <v>95.441024617958405</v>
+      </c>
+      <c r="Q18" s="38">
+        <v>12.258064516129032</v>
+      </c>
+      <c r="S18" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="T18" s="38">
+        <v>16.193548387096776</v>
+      </c>
+      <c r="U18" s="38">
+        <v>20.93548387096774</v>
+      </c>
+      <c r="V18" s="38">
+        <v>2002.9032258064517</v>
+      </c>
+      <c r="W18" s="38">
+        <v>111.96774193548387</v>
+      </c>
+      <c r="X18" s="39">
+        <v>43.60926001088756</v>
+      </c>
+      <c r="Y18" s="39">
+        <v>94.707684024259223</v>
+      </c>
+      <c r="Z18" s="38">
+        <v>11.064516129032258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="38">
+        <v>16.548387096774192</v>
+      </c>
+      <c r="C19" s="38">
+        <v>20.451612903225808</v>
+      </c>
+      <c r="D19" s="38">
+        <v>2013</v>
+      </c>
+      <c r="E19" s="38">
+        <v>102</v>
+      </c>
+      <c r="F19" s="39">
+        <v>44.612340749371739</v>
+      </c>
+      <c r="G19" s="39">
+        <v>95.178815149836439</v>
+      </c>
+      <c r="H19" s="38">
+        <v>11.741935483870968</v>
+      </c>
+      <c r="J19" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="38">
+        <v>16.70967741935484</v>
+      </c>
+      <c r="L19" s="38">
+        <v>20.258064516129032</v>
+      </c>
+      <c r="M19" s="38">
+        <v>2020.3225806451612</v>
+      </c>
+      <c r="N19" s="38">
+        <v>94.709677419354833</v>
+      </c>
+      <c r="O19" s="39">
+        <v>45.153341814371537</v>
+      </c>
+      <c r="P19" s="39">
+        <v>95.523327653158304</v>
+      </c>
+      <c r="Q19" s="38">
+        <v>12.258064516129032</v>
+      </c>
+      <c r="S19" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="T19" s="38">
+        <v>16.032258064516128</v>
+      </c>
+      <c r="U19" s="38">
+        <v>21.06451612903226</v>
+      </c>
+      <c r="V19" s="38">
+        <v>1999.6129032258063</v>
+      </c>
+      <c r="W19" s="38">
+        <v>115.29032258064517</v>
+      </c>
+      <c r="X19" s="39">
+        <v>43.314489970866902</v>
+      </c>
+      <c r="Y19" s="39">
+        <v>94.550851517970969</v>
+      </c>
+      <c r="Z19" s="38">
+        <v>11.129032258064516</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="38">
+        <v>24.483870967741936</v>
+      </c>
+      <c r="C20" s="38">
+        <v>13.096774193548388</v>
+      </c>
+      <c r="D20" s="38">
+        <v>1860.4193548387098</v>
+      </c>
+      <c r="E20" s="38">
+        <v>254</v>
+      </c>
+      <c r="F20" s="39">
+        <v>65.423376854408005</v>
+      </c>
+      <c r="G20" s="39">
+        <v>87.98955867696003</v>
+      </c>
+      <c r="H20" s="38">
+        <v>17.93548387096774</v>
+      </c>
+      <c r="J20" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="38">
+        <v>23.129032258064516</v>
+      </c>
+      <c r="L20" s="38">
+        <v>14.516129032258064</v>
+      </c>
+      <c r="M20" s="38">
+        <v>1905.5806451612902</v>
+      </c>
+      <c r="N20" s="38">
+        <v>208.7741935483871</v>
+      </c>
+      <c r="O20" s="39">
+        <v>61.906966961525526</v>
+      </c>
+      <c r="P20" s="39">
+        <v>90.127957897689825</v>
+      </c>
+      <c r="Q20" s="38">
+        <v>17.096774193548388</v>
+      </c>
+      <c r="S20" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" s="38">
+        <v>26.70967741935484</v>
+      </c>
+      <c r="U20" s="38">
+        <v>11.32258064516129</v>
+      </c>
+      <c r="V20" s="38">
+        <v>1822.258064516129</v>
+      </c>
+      <c r="W20" s="38">
+        <v>291.70967741935482</v>
+      </c>
+      <c r="X20" s="39">
+        <v>70.491031901416775</v>
+      </c>
+      <c r="Y20" s="39">
+        <v>86.203461656902974</v>
+      </c>
+      <c r="Z20" s="38">
+        <v>19.774193548387096</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="S2:Z2"/>
+    <mergeCell ref="S9:Z9"/>
+    <mergeCell ref="S16:Z16"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="J9:Q9"/>
+    <mergeCell ref="J16:Q16"/>
+    <mergeCell ref="J1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>